<commit_message>
fixed some corner case
</commit_message>
<xml_diff>
--- a/reporting/report_template/SBL_CLO_100_Template.xlsx
+++ b/reporting/report_template/SBL_CLO_100_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XiaHanlu\workspace\legacyReporting\reporting\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443C30B1-31BC-4DD8-9CB7-330BC105F1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A46E992-1F02-4088-B256-F447A3BD2A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Disclaimer " sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Disclaimer '!$A$1:$O$35</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Report!$A$1:$S$303</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Report!$A$1:$S$750</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13815" uniqueCount="1650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13814" uniqueCount="1650">
   <si>
     <t>SBL CLO ABS Report</t>
   </si>
@@ -5249,7 +5249,7 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -5369,6 +5369,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5376,6 +5379,105 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="368">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -5992,46 +6094,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="168" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -6053,65 +6115,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="168" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -11502,7 +11505,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_report_manager" displayName="tbl_report_manager" ref="B55:I71" headerRowDxfId="344" dataDxfId="343" totalsRowDxfId="342">
-  <autoFilter ref="B55:I71" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B56:I71">
     <sortCondition descending="1" ref="D55:D71"/>
   </sortState>
@@ -11744,22 +11746,22 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{27E8DB96-6F30-4B07-B6B9-321E95208A1F}" name="Table21" displayName="Table21" ref="N26:R34" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Percent">
-  <autoFilter ref="N26:R33" xr:uid="{27E8DB96-6F30-4B07-B6B9-321E95208A1F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{27E8DB96-6F30-4B07-B6B9-321E95208A1F}" name="Table21" displayName="Table21" ref="N26:R33" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Percent">
+  <autoFilter ref="N26:R32" xr:uid="{27E8DB96-6F30-4B07-B6B9-321E95208A1F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C0E68083-58A0-4469-8380-6EFE6E688032}" name="Collateral Type" totalsRowLabel="Total" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{B110CD2D-60E4-4123-9297-9C7E7830F08A}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{C0E68083-58A0-4469-8380-6EFE6E688032}" name="Collateral Type" totalsRowLabel="Total" dataDxfId="40" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{B110CD2D-60E4-4123-9297-9C7E7830F08A}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="1" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{37038776-57D1-43F8-BD18-FDFAF46F9CD9}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{37038776-57D1-43F8-BD18-FDFAF46F9CD9}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="2" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A8F097ED-132B-4894-8D01-8D0EB3526B1D}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{A8F097ED-132B-4894-8D01-8D0EB3526B1D}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{26DD84D2-9931-4777-99E2-3808183B7A4E}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Percent">
+    <tableColumn id="5" xr3:uid="{26DD84D2-9931-4777-99E2-3808183B7A4E}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</calculatedColumnFormula>
@@ -11770,7 +11772,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="tbl_rawtran" displayName="tbl_rawtran" ref="A1:L64" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="tbl_rawtran" displayName="tbl_rawtran" ref="A1:L64" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A1:L64" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L64">
     <sortCondition ref="D1:D64"/>
@@ -11779,9 +11781,9 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Portfolio"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Security ID"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="Security Description"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Trade Date" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Settle Date" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="Maturity Date" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Trade Date" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Settle Date" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="Maturity Date" dataDxfId="30"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-1000-000008000000}" name="Quantity"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-1000-000009000000}" name="Price"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-1000-00000A000000}" name="Cost Proceeds"/>
@@ -11813,31 +11815,31 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="tbl_rawhold" displayName="tbl_rawhold" ref="A1:V644" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="tbl_rawhold" displayName="tbl_rawhold" ref="A1:V644" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A1:V644" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Portfolio Code" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="CUSIP" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="Current Face" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="BASEMarket Value" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="BASEOriginal Cost" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="Issuer Name" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="Coupon Rate" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1100-000009000000}" name="Security Description" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1100-00000A000000}" name="Maturity Date" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1100-00000B000000}" name="Spread" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1100-00000C000000}" name="Factor" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Yield" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1100-00000D000000}" name="Portfolio_Name" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1100-00000E000000}" name="Row Labels" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1100-00000F000000}" name="Manager" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1100-000010000000}" name="WAL" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1100-000014000000}" name="Implied DM" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-1100-000016000000}" name="Vintage" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1100-000015000000}" name="Collateral Type" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1100-000011000000}" name="Tranche Rating" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1100-000012000000}" name="WAL_Range" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1100-000013000000}" name="coupon_Range" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Portfolio Code" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="CUSIP" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="Current Face" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="BASEMarket Value" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="BASEOriginal Cost" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="Issuer Name" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="Coupon Rate" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1100-000009000000}" name="Security Description" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1100-00000A000000}" name="Maturity Date" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1100-00000B000000}" name="Spread" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1100-00000C000000}" name="Factor" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Yield" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1100-00000D000000}" name="Portfolio_Name" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1100-00000E000000}" name="Row Labels" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1100-00000F000000}" name="Manager" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1100-000010000000}" name="WAL" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1100-000014000000}" name="Implied DM" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-1100-000016000000}" name="Vintage" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1100-000015000000}" name="Collateral Type" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1100-000011000000}" name="Tranche Rating" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1100-000012000000}" name="WAL_Range" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1100-000013000000}" name="coupon_Range" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12907,8 +12909,8 @@
   <dimension ref="B1:S201"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A193" sqref="A193:XFD193"/>
+      <pane ySplit="5" topLeftCell="A739" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B746" sqref="B746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -12959,7 +12961,7 @@
         <v>45869</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1489</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="28" customHeight="1" x14ac:dyDescent="0.6">
@@ -13033,7 +13035,7 @@
       </c>
       <c r="C10" s="24">
         <f>C54</f>
-        <v>1465585847</v>
+        <v>1792045958.5669518</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="17" t="s">
@@ -13051,36 +13053,36 @@
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>3.5821852474534712E-3</v>
+        <v>2.9296123656327852E-3</v>
       </c>
       <c r="I10" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
-        <v>3.5805783310275509E-3</v>
+        <v>2.9797986929207144E-3</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>16</v>
       </c>
       <c r="L10" s="46">
         <f>Table14[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>30.514758</v>
+        <v>181.502526441561</v>
       </c>
       <c r="M10" s="46">
         <f>Table14[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>30.622156499999999</v>
+        <v>175.65110712000001</v>
       </c>
       <c r="N10" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>2.0820860178516722E-2</v>
+        <v>0.10128229444891214</v>
       </c>
       <c r="O10" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>2.081775526736283E-2</v>
+        <v>9.9376286667740801E-2</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
@@ -13089,7 +13091,7 @@
       </c>
       <c r="C11" s="24">
         <f>D54</f>
-        <v>1470963420.7299998</v>
+        <v>1767535425.3000004</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="17" t="s">
@@ -13097,46 +13099,46 @@
       </c>
       <c r="F11" s="47">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>115.497963</v>
+        <v>120.497963</v>
       </c>
       <c r="G11" s="47">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>115.67474282000001</v>
+        <v>120.65678206999999</v>
       </c>
       <c r="H11" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>7.8806685556100348E-2</v>
+        <v>6.7240442369211784E-2</v>
       </c>
       <c r="I11" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
-        <v>7.8638762317144312E-2</v>
+        <v>6.8262723531847258E-2</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>20</v>
       </c>
       <c r="L11" s="46">
         <f>Table14[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>277.85594300000002</v>
+        <v>424.41139310195086</v>
       </c>
       <c r="M11" s="46">
         <f>Table14[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>278.40644864999996</v>
+        <v>409.82270197000008</v>
       </c>
       <c r="N11" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.18958694474892809</v>
+        <v>0.23683064101845949</v>
       </c>
       <c r="O11" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.18926809785102222</v>
+        <v>0.23186109658902121</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
@@ -13147,7 +13149,7 @@
         <f t="array" ref="C12">IFERROR(IF( $C$4 = "All Portfolios",
   SUMPRODUCT( tbl_rawhold[Current Face] *  (tbl_rawhold[Coupon Rate] * 0.01) ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Coupon Rate],"&gt; 0"),
   SUMPRODUCT((tbl_rawhold[Portfolio_Name] = $C$4) *  tbl_rawhold[Current Face] *  (tbl_rawhold[Coupon Rate] * 0.01) ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Coupon Rate],"&gt; 0",tbl_rawhold[Portfolio_Name], $C$4)),0)</f>
-        <v>7.3473126391284074E-2</v>
+        <v>7.1441016616218225E-2</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="17" t="s">
@@ -13155,46 +13157,46 @@
       </c>
       <c r="F12" s="47">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>429.58289000000002</v>
+        <v>441.253722355609</v>
       </c>
       <c r="G12" s="47">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>430.75812534000005</v>
+        <v>441.59184833</v>
       </c>
       <c r="H12" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0.29311342687931946</v>
+        <v>0.2462290212179977</v>
       </c>
       <c r="I12" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
-        <v>0.29284081389748379</v>
+        <v>0.2498347936958884</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="46">
         <f>Table14[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>282.64242200000001</v>
+        <v>383.77552669656001</v>
       </c>
       <c r="M12" s="46">
         <f>Table14[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>285.14680637999993</v>
+        <v>375.77441422999993</v>
       </c>
       <c r="N12" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.1928528598843654</v>
+        <v>0.21415495783570998</v>
       </c>
       <c r="O12" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.19385037204969327</v>
+        <v>0.21259795354099931</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -13205,7 +13207,7 @@
         <f>IFERROR(IF($C$4="All Portfolios",
    SUM(Positions!E:E)/C10,
    SUMIF(Positions!M:M,$C$4,Positions!E:E)/C10),0)</f>
-        <v>1.7964639752078613</v>
+        <v>1.7402396514505953</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="17" t="s">
@@ -13213,46 +13215,46 @@
       </c>
       <c r="F13" s="47">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>2084.7001759999998</v>
+        <v>2310.075090662257</v>
       </c>
       <c r="G13" s="47">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>2091.961214599999</v>
+        <v>2302.270514450001</v>
       </c>
       <c r="H13" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>1.4224347077773056</v>
+        <v>1.2890713430751288</v>
       </c>
       <c r="I13" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
-        <v>1.4221707930451559</v>
+        <v>1.3025314692401375</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>28</v>
       </c>
       <c r="L13" s="46">
         <f>Table14[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>577.44087300000001</v>
+        <v>638.83394442855001</v>
       </c>
       <c r="M13" s="46">
         <f>Table14[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>577.38211272000001</v>
+        <v>633.56747860000041</v>
       </c>
       <c r="N13" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.3940000336261435</v>
+        <v>0.35648301393978055</v>
       </c>
       <c r="O13" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.39251969463214847</v>
+        <v>0.35844683480245731</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
@@ -13261,7 +13263,7 @@
       </c>
       <c r="C14" s="20">
         <f>IFERROR(C11/C10,0)</f>
-        <v>1.0036692314824187</v>
+        <v>0.98632259783864484</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="17" t="s">
@@ -13269,46 +13271,46 @@
       </c>
       <c r="F14" s="47">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>234.07858784198103</v>
       </c>
       <c r="G14" s="47">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>214.66817902999995</v>
       </c>
       <c r="H14" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>0.13062086199461481</v>
       </c>
       <c r="I14" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>0.1214505666801924</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>32</v>
       </c>
       <c r="L14" s="46">
         <f>Table14[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>1455.577033</v>
+        <v>1488.9836150000001</v>
       </c>
       <c r="M14" s="46">
         <f>Table14[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>1461.0674299599993</v>
+        <v>1494.9255546599993</v>
       </c>
       <c r="N14" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.99317077602756076</v>
+        <v>0.83088472585306794</v>
       </c>
       <c r="O14" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.99327244265184422</v>
+        <v>0.84576836948332645</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -13319,7 +13321,7 @@
         <f t="array" ref="C15">IFERROR(IF( $C$4 = "All Portfolios",
   SUMPRODUCT( tbl_rawhold[Current Face]* tbl_rawhold[WAL] ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[WAL],"&gt; 0"),
   SUMPRODUCT((tbl_rawhold[Portfolio_Name] = $C$4) *  tbl_rawhold[Current Face] *  tbl_rawhold[WAL] ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[WAL],"&gt; 0",tbl_rawhold[Portfolio_Name], $C$4)),0)</f>
-        <v>7.4899112648334194</v>
+        <v>6.8734366006368868</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="17" t="s">
@@ -13327,46 +13329,46 @@
       </c>
       <c r="F15" s="47">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>21.376474690810003</v>
       </c>
       <c r="G15" s="47">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>20.7037455</v>
       </c>
       <c r="H15" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>1.1928530397682525E-2</v>
       </c>
       <c r="I15" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>1.1713341188896394E-2</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>36</v>
       </c>
       <c r="L15" s="46">
         <f>Table14[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>4.4950000000000001</v>
       </c>
       <c r="M15" s="46">
         <f>Table14[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>4.5736304499999996</v>
       </c>
       <c r="N15" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>2.5083062063846421E-3</v>
       </c>
       <c r="O15" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>2.5875749840904749E-3</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
@@ -13377,7 +13379,7 @@
         <f t="array" ref="C16">IFERROR(IF( $C$4 = "All Portfolios",
   SUMPRODUCT( tbl_rawhold[Current Face]* tbl_rawhold[Spread] ) /  SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Spread],"&gt; 0"),
   SUMPRODUCT((tbl_rawhold[Portfolio_Name] = $C$4) *  tbl_rawhold[Current Face] *  tbl_rawhold[Spread] ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Spread],"&gt; 0",tbl_rawhold[Portfolio_Name], $C$4)),0)</f>
-        <v>304.51394048622717</v>
+        <v>320.40240329958971</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="17" t="s">
@@ -13385,46 +13387,46 @@
       </c>
       <c r="F16" s="47">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>1.2030000000000001</v>
       </c>
       <c r="G16" s="47">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>0.80212671999999996</v>
       </c>
       <c r="H16" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>6.712997477821411E-4</v>
       </c>
       <c r="I16" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>4.5381083089967293E-4</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>40</v>
       </c>
       <c r="L16" s="46">
         <f>Table14[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>11</v>
+        <v>11.732832882035</v>
       </c>
       <c r="M16" s="46">
         <f>Table14[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>11.0360283</v>
+        <v>11.645208820000001</v>
       </c>
       <c r="N16" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>7.5055309946644158E-3</v>
+        <v>6.5471718657357505E-3</v>
       </c>
       <c r="O16" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>7.5025851387406457E-3</v>
+        <v>6.5883877931462E-3</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
@@ -13435,7 +13437,7 @@
         <f t="array" ref="C17">IFERROR(IF( $C$4 = "All Portfolios",
   SUMPRODUCT( tbl_rawhold[Current Face]* tbl_rawhold[Implied DM] ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Implied DM],"&gt; 0"),
   SUMPRODUCT((tbl_rawhold[Portfolio_Name] = $C$4) *  tbl_rawhold[Current Face] *  tbl_rawhold[Implied DM] ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Implied DM],"&gt; 0",tbl_rawhold[Portfolio_Name], $C$4)),0)</f>
-        <v>298.95829430857657</v>
+        <v>350.95738328101999</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="17" t="s">
@@ -13466,19 +13468,19 @@
       </c>
       <c r="L17" s="46">
         <f>SUBTOTAL(109,Table14[Current Face (M)])</f>
-        <v>2635.0310290000002</v>
+        <v>3133.7348385506566</v>
       </c>
       <c r="M17" s="46">
         <f>SUBTOTAL(109,Table14[Market Value (M)])</f>
-        <v>2643.6609825099995</v>
+        <v>3105.9600958499996</v>
       </c>
       <c r="N17" s="16">
         <f>SUBTOTAL(109,Table14[Portfolio % CF])</f>
-        <v>1.7979370054601789</v>
+        <v>1.7486911111680505</v>
       </c>
       <c r="O17" s="16">
         <f>SUBTOTAL(109,Table14[Portfolio % MV])</f>
-        <v>1.7972309475908117</v>
+        <v>1.7572265038607819</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
@@ -13489,7 +13491,7 @@
         <f t="array" ref="C18">IFERROR(IF( $C$4 = "All Portfolios",
   SUMPRODUCT( tbl_rawhold[Current Face]* tbl_rawhold[Yield] ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Yield],"&gt; 0"),
   SUMPRODUCT((tbl_rawhold[Portfolio_Name] = $C$4) *  tbl_rawhold[Current Face] *  tbl_rawhold[Yield] ) / SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Yield],"&gt; 0",tbl_rawhold[Portfolio_Name], $C$4)),0)</f>
-        <v>7.3458715218459174</v>
+        <v>7.1814734993389191</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="17" t="s">
@@ -13497,19 +13499,19 @@
       </c>
       <c r="F18" s="48">
         <f>SUBTOTAL(109,Table13[Current Face (M)])</f>
-        <v>2635.0310289999998</v>
+        <v>3133.7348385506571</v>
       </c>
       <c r="G18" s="48">
         <f>SUBTOTAL(109,Table13[Market Value (M)])</f>
-        <v>2643.660982509999</v>
+        <v>3105.9600958500009</v>
       </c>
       <c r="H18" s="16">
         <f>SUBTOTAL(109,Table13[Portfolio % CF])</f>
-        <v>1.7979370054601789</v>
+        <v>1.7486911111680508</v>
       </c>
       <c r="I18" s="16">
         <f>SUBTOTAL(109,Table13[Portfolio % MV])</f>
-        <v>1.7972309475908115</v>
+        <v>1.7572265038607822</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
@@ -13518,7 +13520,7 @@
       </c>
       <c r="C19" s="15">
         <f>G54</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="17"/>
@@ -13544,7 +13546,7 @@
       </c>
       <c r="C21" s="15">
         <f>H54</f>
-        <v>183</v>
+        <v>226</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="17"/>
@@ -13629,23 +13631,23 @@
       </c>
       <c r="C27" s="46">
         <f>Table15[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>40.6</v>
+        <v>172.57906060606203</v>
       </c>
       <c r="D27" s="46">
         <f>Table15[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>40.751139500000001</v>
+        <v>157.63821225999996</v>
       </c>
       <c r="E27" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>2.7702232580306844E-2</v>
+        <v>9.6302809523963653E-2</v>
       </c>
       <c r="F27" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>2.7703706921397338E-2</v>
+        <v>8.9185319854760095E-2</v>
       </c>
       <c r="H27" s="17">
         <v>2017</v>
@@ -13662,36 +13664,36 @@
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>5.5438581210589437E-3</v>
+        <v>4.5339238991935968E-3</v>
       </c>
       <c r="L27" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>5.539161793674253E-3</v>
+        <v>4.6097544996118378E-3</v>
       </c>
       <c r="N27" s="17" t="s">
         <v>1524</v>
       </c>
       <c r="O27" s="46">
         <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>4.8109239958999996E-2</v>
       </c>
       <c r="P27" s="46">
         <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>4.7836699999999996E-2</v>
       </c>
       <c r="Q27" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>2.6845985578110726E-5</v>
       </c>
       <c r="R27" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>2.7064068598161626E-5</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
@@ -13700,69 +13702,69 @@
       </c>
       <c r="C28" s="46">
         <f>Table15[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>14.192843110149997</v>
       </c>
       <c r="D28" s="46">
         <f>Table15[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>13.527958649999999</v>
       </c>
       <c r="E28" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>7.9199102245679082E-3</v>
       </c>
       <c r="F28" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>7.6535714398504482E-3</v>
       </c>
       <c r="H28" s="17">
         <v>2018</v>
       </c>
       <c r="I28" s="46">
         <f>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>200.34796299999999</v>
+        <v>209.575963</v>
       </c>
       <c r="J28" s="46">
         <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>200.71752887</v>
+        <v>209.49103614000001</v>
       </c>
       <c r="K28" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.1367016223649436</v>
+        <v>0.11694787290365698</v>
       </c>
       <c r="L28" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.13645310688309928</v>
+        <v>0.11852154878561684</v>
       </c>
       <c r="N28" s="17" t="s">
         <v>1527</v>
       </c>
       <c r="O28" s="46">
         <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P28" s="46">
         <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>7.9699828599999991</v>
       </c>
       <c r="Q28" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>4.4641712238213871E-3</v>
       </c>
       <c r="R28" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>4.509093705234943E-3</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
@@ -13771,23 +13773,23 @@
       </c>
       <c r="C29" s="46">
         <f>Table15[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>54.176261301654002</v>
       </c>
       <c r="D29" s="46">
         <f>Table15[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>52.133453090000003</v>
       </c>
       <c r="E29" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>3.0231513339634003E-2</v>
       </c>
       <c r="F29" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>2.9494997578988547E-2</v>
       </c>
       <c r="H29" s="17">
         <v>2019</v>
@@ -13798,42 +13800,42 @@
       </c>
       <c r="J29" s="46">
         <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>28.817042860000001</v>
+        <v>28.817042860000004</v>
       </c>
       <c r="K29" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>1.9635321983291504E-2</v>
+        <v>1.6058321418839252E-2</v>
       </c>
       <c r="L29" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>1.9590591073773183E-2</v>
+        <v>1.6303516437363025E-2</v>
       </c>
       <c r="N29" s="17" t="s">
         <v>1525</v>
       </c>
       <c r="O29" s="46">
         <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P29" s="46">
         <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>0.90519999999999989</v>
       </c>
       <c r="Q29" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>5.5802140297767338E-4</v>
       </c>
       <c r="R29" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>5.1212552067880735E-4</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
@@ -13842,69 +13844,69 @@
       </c>
       <c r="C30" s="46">
         <f>Table15[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>24.600000000000005</v>
+        <v>124.03283288203498</v>
       </c>
       <c r="D30" s="46">
         <f>Table15[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>26.912182359999999</v>
+        <v>108.48834606</v>
       </c>
       <c r="E30" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>1.6785096588067695E-2</v>
+        <v>6.921297542012847E-2</v>
       </c>
       <c r="F30" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>1.8295616315628163E-2</v>
+        <v>6.13783149730006E-2</v>
       </c>
       <c r="H30" s="17">
         <v>2020</v>
       </c>
       <c r="I30" s="46">
         <f>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>32.44</v>
+        <v>134.447910706838</v>
       </c>
       <c r="J30" s="46">
         <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>32.486228219999994</v>
+        <v>122.69999589999999</v>
       </c>
       <c r="K30" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>2.2134493224264876E-2</v>
+        <v>7.5024811760046703E-2</v>
       </c>
       <c r="L30" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>2.2085000729574873E-2</v>
+        <v>6.9418691214731584E-2</v>
       </c>
       <c r="N30" s="17" t="s">
         <v>1523</v>
       </c>
       <c r="O30" s="46">
         <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="P30" s="46">
         <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>9.3323762100000014</v>
       </c>
       <c r="Q30" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>5.3291043984367813E-3</v>
       </c>
       <c r="R30" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>5.2798807177604568E-3</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
@@ -13923,59 +13925,59 @@
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.50288207648064165</v>
+        <v>0.4112711788872711</v>
       </c>
       <c r="F31" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.50229859636708174</v>
+        <v>0.41801870048211009</v>
       </c>
       <c r="H31" s="17">
         <v>2021</v>
       </c>
       <c r="I31" s="46">
         <f>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>523.67597499999999</v>
+        <v>807.27463803592491</v>
       </c>
       <c r="J31" s="46">
         <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>525.4041612499999</v>
+        <v>787.99578979000046</v>
       </c>
       <c r="K31" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.35731511468396432</v>
+        <v>0.45047652610510031</v>
       </c>
       <c r="L31" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.35718370276621558</v>
+        <v>0.4458161225573487</v>
       </c>
       <c r="N31" s="17" t="s">
         <v>1526</v>
       </c>
       <c r="O31" s="46">
         <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>4.7190395619350003</v>
       </c>
       <c r="P31" s="46">
         <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>4.3788522800000003</v>
       </c>
       <c r="Q31" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>2.633325077058114E-3</v>
       </c>
       <c r="R31" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>2.4773773794416515E-3</v>
       </c>
     </row>
     <row r="32" spans="2:18" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -13984,69 +13986,69 @@
       </c>
       <c r="C32" s="46">
         <f>Table15[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>1832.814175</v>
+        <v>2031.7369866507561</v>
       </c>
       <c r="D32" s="46">
         <f>Table15[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>1837.134799109999</v>
+        <v>2035.3092642500005</v>
       </c>
       <c r="E32" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>1.2505675998111627</v>
+        <v>1.1337527237724854</v>
       </c>
       <c r="F32" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$V$2:$V$644,Table15[[#This Row],[Coupon]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>1.2489330279867041</v>
+        <v>1.1514955995320724</v>
       </c>
       <c r="H32" s="17">
         <v>2022</v>
       </c>
       <c r="I32" s="46">
         <f>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>45.758558000000001</v>
+        <v>47.458557999999996</v>
       </c>
       <c r="J32" s="46">
         <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>45.508681179999996</v>
+        <v>47.150560979999995</v>
       </c>
       <c r="K32" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>3.1222025030922668E-2</v>
+        <v>2.6482891118457287E-2</v>
       </c>
       <c r="L32" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>3.0938010108650601E-2</v>
+        <v>2.6675878913146663E-2</v>
       </c>
       <c r="N32" s="17" t="s">
         <v>1522</v>
       </c>
       <c r="O32" s="46">
         <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
+        <v>40.100505005999999</v>
       </c>
       <c r="P32" s="46">
         <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
+        <v>37.168121200000002</v>
       </c>
       <c r="Q32" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
+        <v>2.2376940063561335E-2</v>
       </c>
       <c r="R32" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
+        <v>2.1028218539773554E-2</v>
       </c>
     </row>
     <row r="33" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -14055,110 +14057,92 @@
       </c>
       <c r="C33" s="46">
         <f>SUBTOTAL(109,Table15[Current Face (M)])</f>
-        <v>2635.0310289999998</v>
+        <v>3133.7348385506571</v>
       </c>
       <c r="D33" s="46">
         <f>SUBTOTAL(109,Table15[Market Value (M)])</f>
-        <v>2643.660982509999</v>
+        <v>3105.9600958500005</v>
       </c>
       <c r="E33" s="16">
         <f>SUBTOTAL(109,Table15[Portfolio % CF])</f>
-        <v>1.7979370054601789</v>
+        <v>1.7486911111680505</v>
       </c>
       <c r="F33" s="16">
         <f>SUBTOTAL(109,Table15[Portfolio % MV])</f>
-        <v>1.7972309475908115</v>
+        <v>1.7572265038607822</v>
       </c>
       <c r="H33" s="17">
         <v>2023</v>
       </c>
       <c r="I33" s="46">
         <f>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>66.611808999999994</v>
+        <v>68.270809</v>
       </c>
       <c r="J33" s="46">
         <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>66.979505770000003</v>
+        <v>68.656142710000012</v>
       </c>
       <c r="K33" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>4.5450636096378734E-2</v>
+        <v>3.8096572620600774E-2</v>
       </c>
       <c r="L33" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>4.553444689791121E-2</v>
+        <v>3.8842866585458748E-2</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>1535</v>
-      </c>
-      <c r="O33" s="46">
-        <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="P33" s="46">
-        <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="20">
-        <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
-   SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0</v>
-      </c>
-      <c r="R33" s="20">
-        <f>IFERROR(IF($C$4="All Portfolios",
-   SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
-   SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="O33" s="53">
+        <f>SUBTOTAL(109,Table21[Current Face (M)])</f>
+        <v>63.417653807893998</v>
+      </c>
+      <c r="P33" s="53">
+        <f>SUBTOTAL(109,Table21[Market Value (M)])</f>
+        <v>59.802369249999998</v>
+      </c>
+      <c r="Q33" s="16">
+        <f>SUBTOTAL(109,Table21[Portfolio % CF])</f>
+        <v>3.5388408151433404E-2</v>
+      </c>
+      <c r="R33" s="16">
+        <f>SUBTOTAL(109,Table21[Portfolio % MV])</f>
+        <v>3.3833759931487573E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" ht="14.5" x14ac:dyDescent="0.35">
       <c r="H34" s="17">
         <v>2024</v>
       </c>
       <c r="I34" s="46">
         <f>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>829.8016100000001</v>
+        <v>830.65161000000001</v>
       </c>
       <c r="J34" s="46">
         <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>833.38076803999991</v>
+        <v>834.23875928999996</v>
       </c>
       <c r="K34" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.56619106393431218</v>
+        <v>0.4635213767978632</v>
       </c>
       <c r="L34" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.56655437945997011</v>
-      </c>
-      <c r="N34" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="O34" s="46">
-        <f>SUBTOTAL(109,Table21[Current Face (M)])</f>
-        <v>0</v>
-      </c>
-      <c r="P34" s="46">
-        <f>SUBTOTAL(109,Table21[Market Value (M)])</f>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="16">
-        <f>SUBTOTAL(109,Table21[Portfolio % CF])</f>
-        <v>0</v>
-      </c>
-      <c r="R34" s="16">
-        <f>SUBTOTAL(109,Table21[Portfolio % MV])</f>
-        <v>0</v>
-      </c>
+        <v>0.47197852294723103</v>
+      </c>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.3">
       <c r="H35" s="17">
@@ -14166,23 +14150,23 @@
       </c>
       <c r="I35" s="46">
         <f>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>899.49286400000017</v>
+        <v>935.73544600000014</v>
       </c>
       <c r="J35" s="46">
         <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>902.21916194000039</v>
+        <v>938.96049455000013</v>
       </c>
       <c r="K35" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>0.61374287002104222</v>
+        <v>0.52216040639285899</v>
       </c>
       <c r="L35" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>0.61335254787794324</v>
+        <v>0.53122584198878631</v>
       </c>
       <c r="N35" s="17"/>
       <c r="O35" s="45"/>
@@ -14196,19 +14180,19 @@
       </c>
       <c r="I36" s="46">
         <f>SUBTOTAL(109,Table20[Current Face (M)])</f>
-        <v>2635.0310290000002</v>
+        <v>3070.3171847427634</v>
       </c>
       <c r="J36" s="46">
         <f>SUBTOTAL(109,Table20[Market Value (M)])</f>
-        <v>2643.6609825100004</v>
+        <v>3046.1577266000004</v>
       </c>
       <c r="K36" s="16">
         <f>SUBTOTAL(109,Table20[Portfolio % CF])</f>
-        <v>1.7979370054601791</v>
+        <v>1.713302703016617</v>
       </c>
       <c r="L36" s="16">
         <f>SUBTOTAL(109,Table20[Portfolio % MV])</f>
-        <v>1.7972309475908124</v>
+        <v>1.7233927439292949</v>
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.3">
@@ -14528,31 +14512,31 @@
       </c>
       <c r="C54" s="6">
         <f>SUM(tbl_report_manager[Current Face])</f>
-        <v>1465585847</v>
+        <v>1792045958.5669518</v>
       </c>
       <c r="D54" s="6">
         <f>SUM(tbl_report_manager[Market Value])</f>
-        <v>1470963420.7299998</v>
+        <v>1767535425.3000004</v>
       </c>
       <c r="E54" s="19">
         <f>SUM(tbl_report_manager[Current Face %])</f>
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="F54" s="19">
         <f>SUM(tbl_report_manager[Market Value %])</f>
-        <v>1.0000000000000002</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="G54" s="21">
         <f>SUM(tbl_report_manager[No. of Issuers])</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H54" s="21">
         <f>SUM(tbl_report_manager[No. of Cusips])</f>
-        <v>183</v>
+        <v>226</v>
       </c>
       <c r="I54" s="21">
         <f>SUM(tbl_report_manager[No. of Positions])</f>
-        <v>225</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.3">
@@ -14589,21 +14573,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>323962871</v>
+        <v>557372676.60031199</v>
       </c>
       <c r="D56" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>326337860.11000001</v>
+        <v>531998804.68999982</v>
       </c>
       <c r="E56" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>0.22104666994645181</v>
+        <v>0.31102588297792716</v>
       </c>
       <c r="F56" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>0.22185314434810843</v>
+        <v>0.30098339024786713</v>
       </c>
       <c r="G56" s="17" cm="1">
         <f t="array" ref="G56">IF($C$4="All Portfolios",
@@ -14617,14 +14601,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="I56" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>30</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14645,11 +14629,11 @@
       </c>
       <c r="E57" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>0.11800297154479822</v>
+        <v>9.6506166135548216E-2</v>
       </c>
       <c r="F57" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>0.1181254872291579</v>
+        <v>9.8305396476287513E-2</v>
       </c>
       <c r="G57" s="17" cm="1">
         <f t="array" ref="G57">IF($C$4="All Portfolios",
@@ -14681,21 +14665,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>127982963</v>
+        <v>129707963</v>
       </c>
       <c r="D58" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>127798818.80999999</v>
+        <v>129486718.70999999</v>
       </c>
       <c r="E58" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>8.7325463235044462E-2</v>
+        <v>7.2379819490636155E-2</v>
       </c>
       <c r="F58" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>8.6881031172465761E-2</v>
+        <v>7.3258344277893309E-2</v>
       </c>
       <c r="G58" s="17" cm="1">
         <f t="array" ref="G58">IF($C$4="All Portfolios",
@@ -14709,14 +14693,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I58" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14727,21 +14711,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>102900000</v>
+        <v>103700000</v>
       </c>
       <c r="D59" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>103345692.30000001</v>
+        <v>104137427.5</v>
       </c>
       <c r="E59" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>7.021083085008803E-2</v>
+        <v>5.7866819488784735E-2</v>
       </c>
       <c r="F59" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>7.0257146332511997E-2</v>
+        <v>5.8916741361675934E-2</v>
       </c>
       <c r="G59" s="17" cm="1">
         <f t="array" ref="G59">IF($C$4="All Portfolios",
@@ -14755,14 +14739,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I59" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.3">
@@ -14773,42 +14757,42 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>42917058</v>
+        <v>102461689.22220601</v>
       </c>
       <c r="D60" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>42519976.659999996</v>
+        <v>100921273.54000001</v>
       </c>
       <c r="E60" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>2.9283209910800946E-2</v>
+        <v>5.7175815571237756E-2</v>
       </c>
       <c r="F60" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>2.8906209400433949E-2</v>
+        <v>5.7097171629740227E-2</v>
       </c>
       <c r="G60" s="17" cm="1">
         <f t="array" ref="G60">IF($C$4="All Portfolios",
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$F$2:$F$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$F$2:$F$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H60" s="17" cm="1">
         <f t="array" ref="H60">IF($C$4="All Portfolios",
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I60" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.3">
@@ -14819,21 +14803,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>90418501</v>
+        <v>93016501</v>
       </c>
       <c r="D61" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>90420622.659999996</v>
+        <v>92565340.939999998</v>
       </c>
       <c r="E61" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>6.1694441976963221E-2</v>
+        <v>5.1905198388094161E-2</v>
       </c>
       <c r="F61" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>6.1470340720727552E-2</v>
+        <v>5.2369723183505107E-2</v>
       </c>
       <c r="G61" s="17" cm="1">
         <f t="array" ref="G61">IF($C$4="All Portfolios",
@@ -14847,14 +14831,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I61" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.3">
@@ -14865,21 +14849,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>77212000</v>
+        <v>77462000</v>
       </c>
       <c r="D62" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>77550198.410000011</v>
+        <v>77803793.910000011</v>
       </c>
       <c r="E62" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>5.2683369014548079E-2</v>
+        <v>4.3225453917456538E-2</v>
       </c>
       <c r="F62" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>5.2720684496364925E-2</v>
+        <v>4.4018237369581728E-2</v>
       </c>
       <c r="G62" s="17" cm="1">
         <f t="array" ref="G62">IF($C$4="All Portfolios",
@@ -14893,14 +14877,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I62" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14911,21 +14895,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>51466730</v>
+        <v>74904404.744433999</v>
       </c>
       <c r="D63" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>51605900.039999999</v>
+        <v>74467667.170000002</v>
       </c>
       <c r="E63" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>3.5116830655365902E-2</v>
+        <v>4.1798261024696554E-2</v>
       </c>
       <c r="F63" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>3.5083061422689472E-2</v>
+        <v>4.213079189479936E-2</v>
       </c>
       <c r="G63" s="17" cm="1">
         <f t="array" ref="G63">IF($C$4="All Portfolios",
@@ -14939,14 +14923,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I63" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.3">
@@ -14957,21 +14941,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>69035823</v>
+        <v>70255823</v>
       </c>
       <c r="D64" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>69211097.379999995</v>
+        <v>70471703.699999988</v>
       </c>
       <c r="E64" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>4.7104591751696956E-2</v>
+        <v>3.9204252917811093E-2</v>
       </c>
       <c r="F64" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>4.7051542142123683E-2</v>
+        <v>3.987003750605958E-2</v>
       </c>
       <c r="G64" s="17" cm="1">
         <f t="array" ref="G64">IF($C$4="All Portfolios",
@@ -14985,14 +14969,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I64" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15013,11 +14997,11 @@
       </c>
       <c r="E65" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>4.6510410931936357E-2</v>
+        <v>3.8037528933973108E-2</v>
       </c>
       <c r="F65" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>4.6571676280027882E-2</v>
+        <v>3.8757487555516876E-2</v>
       </c>
       <c r="G65" s="17" cm="1">
         <f t="array" ref="G65">IF($C$4="All Portfolios",
@@ -15049,21 +15033,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>65196000</v>
+        <v>67496000</v>
       </c>
       <c r="D66" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>65393983.579999998</v>
+        <v>67720521.980000004</v>
       </c>
       <c r="E66" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>4.4484599884376474E-2</v>
+        <v>3.7664212615381047E-2</v>
       </c>
       <c r="F66" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>4.4456566804051939E-2</v>
+        <v>3.8313530247070397E-2</v>
       </c>
       <c r="G66" s="17" cm="1">
         <f t="array" ref="G66">IF($C$4="All Portfolios",
@@ -15077,14 +15061,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I66" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
@@ -15095,21 +15079,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>66537000</v>
+        <v>66637000</v>
       </c>
       <c r="D67" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>66913550.850000001</v>
+        <v>67014235.649999999</v>
       </c>
       <c r="E67" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>4.5399592344726021E-2</v>
+        <v>3.7184872230223223E-2</v>
       </c>
       <c r="F67" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>4.5489608991631209E-2</v>
+        <v>3.7913942029549876E-2</v>
       </c>
       <c r="G67" s="17" cm="1">
         <f t="array" ref="G67">IF($C$4="All Portfolios",
@@ -15123,14 +15107,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I67" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -15151,11 +15135,11 @@
       </c>
       <c r="E68" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>3.7664119173225069E-2</v>
+        <v>3.0802781444367572E-2</v>
       </c>
       <c r="F68" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>3.7637210837319704E-2</v>
+        <v>3.1322122095857489E-2</v>
       </c>
       <c r="G68" s="17" cm="1">
         <f t="array" ref="G68">IF($C$4="All Portfolios",
@@ -15187,21 +15171,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>52569619</v>
+        <v>53144619</v>
       </c>
       <c r="D69" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>52825042.079999998</v>
+        <v>53403021.159999996</v>
       </c>
       <c r="E69" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>3.5869354980199941E-2</v>
+        <v>2.9655834855093918E-2</v>
       </c>
       <c r="F69" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>3.5911866560070095E-2</v>
+        <v>3.0213267805331824E-2</v>
       </c>
       <c r="G69" s="17" cm="1">
         <f t="array" ref="G69">IF($C$4="All Portfolios",
@@ -15215,14 +15199,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I69" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -15233,21 +15217,21 @@
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>50328267</v>
+        <v>50828267</v>
       </c>
       <c r="D70" s="10">
         <f>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</f>
-        <v>50484857.25</v>
+        <v>50989095.75</v>
       </c>
       <c r="E70" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>3.4340033443295115E-2</v>
+        <v>2.8363260862263779E-2</v>
       </c>
       <c r="F70" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>3.4320946760828162E-2</v>
+        <v>2.8847566515588063E-2</v>
       </c>
       <c r="G70" s="17" cm="1">
         <f t="array" ref="G70">IF($C$4="All Portfolios",
@@ -15261,14 +15245,14 @@
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I70" s="17">
         <f>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
 )</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
@@ -15289,11 +15273,11 @@
       </c>
       <c r="E71" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</f>
-        <v>3.3263510356483401E-2</v>
+        <v>2.7203839146505156E-2</v>
       </c>
       <c r="F71" s="20">
         <f>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</f>
-        <v>3.3263476501487484E-2</v>
+        <v>2.7682249803675254E-2</v>
       </c>
       <c r="G71" s="17" cm="1">
         <f t="array" ref="G71">IF($C$4="All Portfolios",
@@ -17780,7 +17764,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated Template and added portfolios to Skyridge
</commit_message>
<xml_diff>
--- a/reporting/report_template/SBL_CLO_100_Template.xlsx
+++ b/reporting/report_template/SBL_CLO_100_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XiaHanlu\workspace\legacyReporting\reporting\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3103A155-7275-4B5C-A95D-BA5128366133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC783897-2FA0-4B08-B7B2-9ED0BAC2019C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13814" uniqueCount="1650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13815" uniqueCount="1652">
   <si>
     <t>SBL CLO ABS Report</t>
   </si>
@@ -5014,6 +5014,12 @@
   </si>
   <si>
     <t>Market Value (M)</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>PC Rated Feeder</t>
   </si>
 </sst>
 </file>
@@ -5115,7 +5121,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5138,6 +5144,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF5DBAFF"/>
         <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="65"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -5249,7 +5261,7 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -5351,9 +5363,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -5364,6 +5373,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5378,7 +5393,132 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="368">
+  <dxfs count="366">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -5995,28 +6135,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6036,86 +6156,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="168" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6271,7 +6312,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6295,7 +6337,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6314,7 +6356,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6338,7 +6381,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -7176,8 +7219,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
@@ -7191,7 +7232,14 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -7215,50 +7263,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -7444,7 +7449,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -7487,7 +7492,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -11458,33 +11463,33 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleEldridge" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="367"/>
-      <tableStyleElement type="headerRow" dxfId="366"/>
-      <tableStyleElement type="totalRow" dxfId="365"/>
-      <tableStyleElement type="firstColumn" dxfId="364"/>
-      <tableStyleElement type="lastColumn" dxfId="363"/>
-      <tableStyleElement type="firstRowStripe" dxfId="362"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="361"/>
+      <tableStyleElement type="wholeTable" dxfId="365"/>
+      <tableStyleElement type="headerRow" dxfId="364"/>
+      <tableStyleElement type="totalRow" dxfId="363"/>
+      <tableStyleElement type="firstColumn" dxfId="362"/>
+      <tableStyleElement type="lastColumn" dxfId="361"/>
+      <tableStyleElement type="firstRowStripe" dxfId="360"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="359"/>
     </tableStyle>
     <tableStyle name="TableStyleEldridge2" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="360"/>
-      <tableStyleElement type="headerRow" dxfId="359"/>
-      <tableStyleElement type="totalRow" dxfId="358"/>
-      <tableStyleElement type="firstColumn" dxfId="357"/>
-      <tableStyleElement type="lastColumn" dxfId="356"/>
-      <tableStyleElement type="firstRowStripe" dxfId="355"/>
-      <tableStyleElement type="secondRowStripe" dxfId="354"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="353"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="352"/>
+      <tableStyleElement type="wholeTable" dxfId="358"/>
+      <tableStyleElement type="headerRow" dxfId="357"/>
+      <tableStyleElement type="totalRow" dxfId="356"/>
+      <tableStyleElement type="firstColumn" dxfId="355"/>
+      <tableStyleElement type="lastColumn" dxfId="354"/>
+      <tableStyleElement type="firstRowStripe" dxfId="353"/>
+      <tableStyleElement type="secondRowStripe" dxfId="352"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="351"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="350"/>
     </tableStyle>
     <tableStyle name="TableStyleEldridge3" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="wholeTable" dxfId="351"/>
-      <tableStyleElement type="headerRow" dxfId="350"/>
-      <tableStyleElement type="totalRow" dxfId="349"/>
-      <tableStyleElement type="firstColumn" dxfId="348"/>
-      <tableStyleElement type="lastColumn" dxfId="347"/>
-      <tableStyleElement type="firstRowStripe" dxfId="346"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="345"/>
+      <tableStyleElement type="wholeTable" dxfId="349"/>
+      <tableStyleElement type="headerRow" dxfId="348"/>
+      <tableStyleElement type="totalRow" dxfId="347"/>
+      <tableStyleElement type="firstColumn" dxfId="346"/>
+      <tableStyleElement type="lastColumn" dxfId="345"/>
+      <tableStyleElement type="firstRowStripe" dxfId="344"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="343"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -11504,41 +11509,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_report_manager" displayName="tbl_report_manager" ref="B55:I71" headerRowDxfId="344" dataDxfId="343" totalsRowDxfId="342">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tbl_report_manager" displayName="tbl_report_manager" ref="B55:I71" headerRowDxfId="342" dataDxfId="341" totalsRowDxfId="340">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B56:I71">
     <sortCondition descending="1" ref="D55:D71"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Manager Name" totalsRowLabel="Total" dataDxfId="341" totalsRowDxfId="340"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Current Face" dataDxfId="339" totalsRowDxfId="338" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Manager Name" totalsRowLabel="Total" dataDxfId="339" totalsRowDxfId="338"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Current Face" dataDxfId="337" totalsRowDxfId="336" dataCellStyle="Comma">
       <calculatedColumnFormula>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[Current Face], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Market Value" dataDxfId="337" totalsRowDxfId="336" dataCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Market Value" dataDxfId="335" totalsRowDxfId="334" dataCellStyle="Comma">
       <calculatedColumnFormula>IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]),
    SUMIFS(tbl_rawhold[BASEMarket Value], tbl_rawhold[Portfolio_Name], $C$4,tbl_rawhold[Manager], tbl_report_manager[[#This Row],[Manager Name]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Current Face %" dataDxfId="335" totalsRowDxfId="334" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Current Face %" dataDxfId="333" totalsRowDxfId="332" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(tbl_report_manager[[#This Row],[Current Face]]/$C$54,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Market Value %" dataDxfId="333" totalsRowDxfId="332" dataCellStyle="Percent">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Market Value %" dataDxfId="331" totalsRowDxfId="330" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(tbl_report_manager[[#This Row],[Market Value]]/$D$54,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. of Issuers" dataDxfId="331">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. of Issuers" dataDxfId="329">
       <calculatedColumnFormula array="1">IF($C$4="All Portfolios",
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$F$2:$F$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$F$2:$F$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No. of Cusips" dataDxfId="330" totalsRowDxfId="329">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="No. of Cusips" dataDxfId="328" totalsRowDxfId="327">
       <calculatedColumnFormula array="1">IF($C$4="All Portfolios",
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]]))),0),
    IFERROR(ROWS(_xlfn.UNIQUE(_xlfn._xlws.FILTER(Positions!$B$2:$B$644, (Positions!$O$2:$O$644=tbl_report_manager[[#This Row],[Manager Name]])*(Positions!$M$2:$M$644=$C$4)))),0)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="No. of Positions" totalsRowFunction="sum" dataDxfId="328" totalsRowDxfId="327">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="No. of Positions" totalsRowFunction="sum" dataDxfId="326" totalsRowDxfId="325">
       <calculatedColumnFormula>IF($C$4="All Portfolios",
    COUNTIFS(Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]]),
    COUNTIFS(Positions!$M$2:$M$644, $C$4,Positions!$O$2:$O$644, tbl_report_manager[[#This Row],[Manager Name]])
@@ -11550,60 +11555,60 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="tbl_hold_b" displayName="tbl_hold_b" ref="B182:S185" totalsRowShown="0" headerRowDxfId="159" dataDxfId="158">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="tbl_hold_b" displayName="tbl_hold_b" ref="B182:S185" totalsRowShown="0" headerRowDxfId="157" dataDxfId="156">
   <autoFilter ref="B182:S185" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Cusip" dataDxfId="157"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Issuer" dataDxfId="156"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Security Description" dataDxfId="155"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Issue Date" dataDxfId="154"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Maturity Date" dataDxfId="153"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Coupon" dataDxfId="152"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="Spread" dataDxfId="151"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="Current Face" dataDxfId="150" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="Factor" dataDxfId="149"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Market Price" dataDxfId="148"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="Market Value" dataDxfId="147" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="NRSRO" dataDxfId="146"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0900-00000D000000}" name="NRSRO Rating" dataDxfId="145"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="WAL" dataDxfId="144"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="Par Sub" dataDxfId="143" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0900-000010000000}" name="Implied DM" dataDxfId="142"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0900-000011000000}" name="Next Payment Date" dataDxfId="141"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0900-000012000000}" name="Non-Call Date" dataDxfId="140"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Cusip" dataDxfId="155"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Issuer" dataDxfId="154"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Security Description" dataDxfId="153"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Issue Date" dataDxfId="152"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Maturity Date" dataDxfId="151"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Coupon" dataDxfId="150"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="Spread" dataDxfId="149"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="Current Face" dataDxfId="148" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="Factor" dataDxfId="147"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="Market Price" dataDxfId="146"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="Market Value" dataDxfId="145" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="NRSRO" dataDxfId="144"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0900-00000D000000}" name="NRSRO Rating" dataDxfId="143"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="WAL" dataDxfId="142"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="Par Sub" dataDxfId="141" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0900-000010000000}" name="Implied DM" dataDxfId="140"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0900-000011000000}" name="Next Payment Date" dataDxfId="139"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0900-000012000000}" name="Non-Call Date" dataDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table11" displayName="Table11" ref="B9:C21" totalsRowShown="0" headerRowDxfId="139" dataDxfId="138">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table11" displayName="Table11" ref="B9:C21" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
   <autoFilter ref="B9:C21" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Characteristics" dataDxfId="137"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Total" dataDxfId="136"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Characteristics" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Total" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table13" displayName="Table13" ref="E9:I18" totalsRowCount="1" headerRowDxfId="135" dataDxfId="134" totalsRowDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table13" displayName="Table13" ref="E9:I18" totalsRowCount="1" headerRowDxfId="133" dataDxfId="132" totalsRowDxfId="131">
   <autoFilter ref="E9:I17" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Tranche Rating" totalsRowLabel="Total" dataDxfId="132" totalsRowDxfId="131"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="130" totalsRowDxfId="129" dataCellStyle="Percent" totalsRowCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Tranche Rating" totalsRowLabel="Total" dataDxfId="130" totalsRowDxfId="129"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="128" totalsRowDxfId="127" dataCellStyle="Percent" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="128" totalsRowDxfId="127" dataCellStyle="Percent" totalsRowCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="126" totalsRowDxfId="125" dataCellStyle="Percent" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{54C6FBDC-154E-4D7B-BF3C-D3F0A98C1B16}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="126" totalsRowDxfId="125" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{54C6FBDC-154E-4D7B-BF3C-D3F0A98C1B16}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="124" totalsRowDxfId="123" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$10,
    SUMIFS(tbl_rawhold[Current Face],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$10),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{775CE8B0-79E2-4AC4-8CB8-D7067A620237}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="124" totalsRowDxfId="123" dataCellStyle="Percent">
+    <tableColumn id="5" xr3:uid="{775CE8B0-79E2-4AC4-8CB8-D7067A620237}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="122" totalsRowDxfId="121" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]])/$C$11,
    SUMIFS(tbl_rawhold[BASEMarket Value],tbl_rawhold[Tranche Rating],Table13[[#This Row],[Tranche Rating]],tbl_rawhold[Portfolio_Name],$C$4)/$C$11),0)</calculatedColumnFormula>
@@ -11614,22 +11619,22 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table14" displayName="Table14" ref="K9:O17" totalsRowCount="1" headerRowDxfId="122" dataDxfId="121" totalsRowDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table14" displayName="Table14" ref="K9:O17" totalsRowCount="1" headerRowDxfId="120" dataDxfId="119" totalsRowDxfId="118">
   <autoFilter ref="K9:O16" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="WAL" totalsRowLabel="Total" dataDxfId="119" totalsRowDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="117" totalsRowDxfId="116" dataCellStyle="Percent" totalsRowCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="WAL" totalsRowLabel="Total" dataDxfId="117" totalsRowDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="115" totalsRowDxfId="114" dataCellStyle="Percent" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>Table14[[#This Row],[Portfolio % CF]]*$C$10/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="115" totalsRowDxfId="114" dataCellStyle="Percent" totalsRowCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112" dataCellStyle="Percent" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>Table14[[#This Row],[Portfolio % MV]]*$C$11/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D8C00212-BAA8-4A57-BCC8-B6A723F048FC}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{D8C00212-BAA8-4A57-BCC8-B6A723F048FC}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="111" totalsRowDxfId="110" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6F65F161-D1CD-406E-9006-86D0A0BA1B26}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="111" totalsRowDxfId="110" dataCellStyle="Percent">
+    <tableColumn id="5" xr3:uid="{6F65F161-D1CD-406E-9006-86D0A0BA1B26}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="109" totalsRowDxfId="108" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,Positions!$U$2:$U$644,Table14[[#This Row],[WAL]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</calculatedColumnFormula>
@@ -11640,14 +11645,14 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table15" displayName="Table15" ref="B26:F33" totalsRowCount="1" headerRowDxfId="109" dataDxfId="108" totalsRowDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table15" displayName="Table15" ref="B26:F33" totalsRowCount="1" headerRowDxfId="107" dataDxfId="106" totalsRowDxfId="105">
   <autoFilter ref="B26:F32" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Coupon" totalsRowLabel="Total" dataDxfId="106" totalsRowDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="104" totalsRowDxfId="103" dataCellStyle="Percent" totalsRowCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Coupon" totalsRowLabel="Total" dataDxfId="104" totalsRowDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="102" dataCellStyle="Percent" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>Table15[[#This Row],[Portfolio % CF]]*$C$10/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="102" totalsRowDxfId="101" dataCellStyle="Percent" totalsRowCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="101" dataCellStyle="Percent" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>Table15[[#This Row],[Portfolio % MV]]*$C$11/1000000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{56192596-1701-43CC-9257-DACFDC295352}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="100" totalsRowDxfId="99" dataCellStyle="Percent">
@@ -11720,14 +11725,14 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{12D42117-5193-441A-8C14-66A40D5E97B1}" name="Table20" displayName="Table20" ref="H26:L36" totalsRowCount="1" headerRowDxfId="56" dataDxfId="55" totalsRowDxfId="54">
-  <autoFilter ref="H26:L35" xr:uid="{12D42117-5193-441A-8C14-66A40D5E97B1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{12D42117-5193-441A-8C14-66A40D5E97B1}" name="Table20" displayName="Table20" ref="H26:L37" totalsRowCount="1" headerRowDxfId="56" dataDxfId="55" totalsRowDxfId="54">
+  <autoFilter ref="H26:L36" xr:uid="{12D42117-5193-441A-8C14-66A40D5E97B1}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2727D7D5-D5F7-4EE8-96FD-6A1A9AB27A40}" name="Vintage" totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{C11EED73-564D-45E3-BA47-0F6B94FCFA00}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50" dataCellStyle="Percent" totalsRowCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{C11EED73-564D-45E3-BA47-0F6B94FCFA00}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="51" totalsRowDxfId="50" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9A8F8B71-DCBA-41AB-9C93-D8D1AA49B14C}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48" dataCellStyle="Percent" totalsRowCellStyle="Comma">
+    <tableColumn id="3" xr3:uid="{9A8F8B71-DCBA-41AB-9C93-D8D1AA49B14C}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{18762466-9940-404E-B47A-2FC91F086CD5}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="46" dataCellStyle="Percent">
@@ -11749,19 +11754,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{27E8DB96-6F30-4B07-B6B9-321E95208A1F}" name="Table21" displayName="Table21" ref="N26:R33" totalsRowCount="1" headerRowDxfId="43" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Percent">
   <autoFilter ref="N26:R32" xr:uid="{27E8DB96-6F30-4B07-B6B9-321E95208A1F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C0E68083-58A0-4469-8380-6EFE6E688032}" name="Collateral Type" totalsRowLabel="Total" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{B110CD2D-60E4-4123-9297-9C7E7830F08A}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{C0E68083-58A0-4469-8380-6EFE6E688032}" name="Collateral Type" totalsRowLabel="Total" dataDxfId="40" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B110CD2D-60E4-4123-9297-9C7E7830F08A}" name="Current Face (M)" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{37038776-57D1-43F8-BD18-FDFAF46F9CD9}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="3" xr3:uid="{37038776-57D1-43F8-BD18-FDFAF46F9CD9}" name="Market Value (M)" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="2" dataCellStyle="Percent">
       <calculatedColumnFormula>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A8F097ED-132B-4894-8D01-8D0EB3526B1D}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{A8F097ED-132B-4894-8D01-8D0EB3526B1D}" name="Portfolio % CF" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{26DD84D2-9931-4777-99E2-3808183B7A4E}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Percent">
+    <tableColumn id="5" xr3:uid="{26DD84D2-9931-4777-99E2-3808183B7A4E}" name="Portfolio % MV" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="0" dataCellStyle="Percent">
       <calculatedColumnFormula>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</calculatedColumnFormula>
@@ -11772,7 +11777,7 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="tbl_rawtran" displayName="tbl_rawtran" ref="A1:L64" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="tbl_rawtran" displayName="tbl_rawtran" ref="A1:L64" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A1:L64" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L64">
     <sortCondition ref="D1:D64"/>
@@ -11781,9 +11786,9 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Portfolio"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Security ID"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="Security Description"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Trade Date" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Settle Date" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="Maturity Date" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Trade Date" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Settle Date" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="Maturity Date" dataDxfId="30"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-1000-000008000000}" name="Quantity"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-1000-000009000000}" name="Price"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-1000-00000A000000}" name="Cost Proceeds"/>
@@ -11796,236 +11801,236 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tbl_report_paydown" displayName="tbl_report_paydown" ref="B78:H80" totalsRowShown="0" headerRowDxfId="326" dataDxfId="325">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tbl_report_paydown" displayName="tbl_report_paydown" ref="B78:H80" totalsRowShown="0" headerRowDxfId="324" dataDxfId="323">
   <autoFilter ref="B78:H80" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B79:H80">
     <sortCondition ref="F78:F80"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Type" dataDxfId="324"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Issuer" dataDxfId="323"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Security Description" dataDxfId="322"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Cusip" dataDxfId="321"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Settle Date" dataDxfId="320"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Face Value" dataDxfId="319" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Tranche Rating" dataDxfId="318"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Type" dataDxfId="322"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Issuer" dataDxfId="321"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Security Description" dataDxfId="320"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Cusip" dataDxfId="319"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Settle Date" dataDxfId="318"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Face Value" dataDxfId="317" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Tranche Rating" dataDxfId="316"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="tbl_rawhold" displayName="tbl_rawhold" ref="A1:V644" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="tbl_rawhold" displayName="tbl_rawhold" ref="A1:V644" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A1:V644" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}"/>
   <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Portfolio Code" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="CUSIP" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="Current Face" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="BASEMarket Value" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="BASEOriginal Cost" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="Issuer Name" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="Coupon Rate" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1100-000009000000}" name="Security Description" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1100-00000A000000}" name="Maturity Date" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1100-00000B000000}" name="Spread" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1100-00000C000000}" name="Factor" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Yield" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1100-00000D000000}" name="Portfolio_Name" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1100-00000E000000}" name="Row Labels" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1100-00000F000000}" name="Manager" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1100-000010000000}" name="WAL" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1100-000014000000}" name="Implied DM" dataDxfId="5"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-1100-000016000000}" name="Vintage" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1100-000015000000}" name="Collateral Type" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1100-000011000000}" name="Tranche Rating" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1100-000012000000}" name="WAL_Range" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1100-000013000000}" name="coupon_Range" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Portfolio Code" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="CUSIP" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="Current Face" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="BASEMarket Value" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="BASEOriginal Cost" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1100-000007000000}" name="Issuer Name" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-1100-000008000000}" name="Coupon Rate" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-1100-000009000000}" name="Security Description" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-1100-00000A000000}" name="Maturity Date" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1100-00000B000000}" name="Spread" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-1100-00000C000000}" name="Factor" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Yield" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-1100-00000D000000}" name="Portfolio_Name" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-1100-00000E000000}" name="Row Labels" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-1100-00000F000000}" name="Manager" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-1100-000010000000}" name="WAL" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-1100-000014000000}" name="Implied DM" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-1100-000016000000}" name="Vintage" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-1100-000015000000}" name="Collateral Type" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-1100-000011000000}" name="Tranche Rating" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-1100-000012000000}" name="WAL_Range" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-1100-000013000000}" name="coupon_Range" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tbl_report_sale" displayName="tbl_report_sale" ref="B86:J87" totalsRowShown="0" headerRowDxfId="317" dataDxfId="316">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tbl_report_sale" displayName="tbl_report_sale" ref="B86:J87" totalsRowShown="0" headerRowDxfId="315" dataDxfId="314">
   <autoFilter ref="B86:J87" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Issuer" dataDxfId="315"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Security Description" dataDxfId="314"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cusip" dataDxfId="313"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Trade Date" dataDxfId="312"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Settle Date" dataDxfId="311"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Face Value" dataDxfId="310" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Sale Price" dataDxfId="309"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Maturity Date" dataDxfId="308"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Tranche Rating" dataDxfId="307"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Issuer" dataDxfId="313"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Security Description" dataDxfId="312"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cusip" dataDxfId="311"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Trade Date" dataDxfId="310"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Settle Date" dataDxfId="309"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Face Value" dataDxfId="308" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Sale Price" dataDxfId="307"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Maturity Date" dataDxfId="306"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Tranche Rating" dataDxfId="305"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tbl_report_purchase" displayName="tbl_report_purchase" ref="B94:J96" totalsRowShown="0" headerRowDxfId="306" dataDxfId="305">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tbl_report_purchase" displayName="tbl_report_purchase" ref="B94:J96" totalsRowShown="0" headerRowDxfId="304" dataDxfId="303">
   <autoFilter ref="B94:J96" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B95:J96">
     <sortCondition ref="E94:E96"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Issuer" dataDxfId="304"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Security Description" dataDxfId="303"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Cusip" dataDxfId="302"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Trade Date" dataDxfId="301"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Settle Date" dataDxfId="300"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Face Value" dataDxfId="299" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Purchase Price" dataDxfId="298" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Maturity Date" dataDxfId="297"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Tranche Rating" dataDxfId="296"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Issuer" dataDxfId="302"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Security Description" dataDxfId="301"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Cusip" dataDxfId="300"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Trade Date" dataDxfId="299"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Settle Date" dataDxfId="298"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Face Value" dataDxfId="297" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Purchase Price" dataDxfId="296" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Maturity Date" dataDxfId="295"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Tranche Rating" dataDxfId="294"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tbl_hold_aaa" displayName="tbl_hold_aaa" ref="B103:S104" headerRowDxfId="295" dataDxfId="294" totalsRowDxfId="293">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tbl_hold_aaa" displayName="tbl_hold_aaa" ref="B103:S104" headerRowDxfId="293" dataDxfId="292" totalsRowDxfId="291">
   <autoFilter ref="B103:S104" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Cusip" totalsRowLabel="Total" dataDxfId="292" totalsRowDxfId="291"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Issuer" dataDxfId="290" totalsRowDxfId="289"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Security Description" dataDxfId="288" totalsRowDxfId="287"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Issue Date" dataDxfId="286" totalsRowDxfId="285"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Maturity Date" dataDxfId="284" totalsRowDxfId="283"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Coupon" dataDxfId="282" totalsRowDxfId="281"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Spread" dataDxfId="280" totalsRowDxfId="279"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Current Face" dataDxfId="278" totalsRowDxfId="277" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Factor" dataDxfId="276" totalsRowDxfId="275"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Market Price" dataDxfId="274" totalsRowDxfId="273"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Market Value" dataDxfId="272" totalsRowDxfId="271" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="NRSRO" dataDxfId="270" totalsRowDxfId="269"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="NRSRO Rating" dataDxfId="268" totalsRowDxfId="267"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="WAL" dataDxfId="266" totalsRowDxfId="265"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="Par Sub" dataDxfId="264" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="Implied DM" dataDxfId="263" totalsRowDxfId="262"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="Next Payment Date" dataDxfId="261" totalsRowDxfId="260"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="Non-Call Date" totalsRowFunction="count" dataDxfId="259" totalsRowDxfId="258"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Cusip" totalsRowLabel="Total" dataDxfId="290" totalsRowDxfId="289"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Issuer" dataDxfId="288" totalsRowDxfId="287"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Security Description" dataDxfId="286" totalsRowDxfId="285"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Issue Date" dataDxfId="284" totalsRowDxfId="283"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Maturity Date" dataDxfId="282" totalsRowDxfId="281"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Coupon" dataDxfId="280" totalsRowDxfId="279"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Spread" dataDxfId="278" totalsRowDxfId="277"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Current Face" dataDxfId="276" totalsRowDxfId="275" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Factor" dataDxfId="274" totalsRowDxfId="273"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Market Price" dataDxfId="272" totalsRowDxfId="271"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Market Value" dataDxfId="270" totalsRowDxfId="269" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="NRSRO" dataDxfId="268" totalsRowDxfId="267"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="NRSRO Rating" dataDxfId="266" totalsRowDxfId="265"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="WAL" dataDxfId="264" totalsRowDxfId="263"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="Par Sub" dataDxfId="262" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="Implied DM" dataDxfId="261" totalsRowDxfId="260"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0400-000011000000}" name="Next Payment Date" dataDxfId="259" totalsRowDxfId="258"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="Non-Call Date" totalsRowFunction="count" dataDxfId="257" totalsRowDxfId="256"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tbl_hold_aa" displayName="tbl_hold_aa" ref="B111:S117" totalsRowShown="0" headerRowDxfId="257" dataDxfId="256">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tbl_hold_aa" displayName="tbl_hold_aa" ref="B111:S117" totalsRowShown="0" headerRowDxfId="255" dataDxfId="254">
   <autoFilter ref="B111:S117" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B112:S117">
     <sortCondition ref="C111:C117"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Cusip" dataDxfId="255"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Issuer" dataDxfId="254"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Security Description" dataDxfId="253"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Issue Date" dataDxfId="252"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Maturity Date" dataDxfId="251"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Coupon" dataDxfId="250"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Spread" dataDxfId="249"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Current Face" dataDxfId="248" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Factor" dataDxfId="247"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Market Price" dataDxfId="246"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="Market Value" dataDxfId="245" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NRSRO" dataDxfId="244"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="NRSRO Rating" dataDxfId="243"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="WAL" dataDxfId="242"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Par Sub" dataDxfId="241"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Implied DM" dataDxfId="240"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Next Payment Date" dataDxfId="239"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="Non-Call Date" dataDxfId="238"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Cusip" dataDxfId="253"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Issuer" dataDxfId="252"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Security Description" dataDxfId="251"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Issue Date" dataDxfId="250"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Maturity Date" dataDxfId="249"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Coupon" dataDxfId="248"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Spread" dataDxfId="247"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Current Face" dataDxfId="246" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Factor" dataDxfId="245"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="Market Price" dataDxfId="244"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="Market Value" dataDxfId="243" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NRSRO" dataDxfId="242"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="NRSRO Rating" dataDxfId="241"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="WAL" dataDxfId="240"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Par Sub" dataDxfId="239"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Implied DM" dataDxfId="238"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Next Payment Date" dataDxfId="237"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="Non-Call Date" dataDxfId="236"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tbl_hold_a" displayName="tbl_hold_a" ref="B124:S135" headerRowDxfId="237" dataDxfId="236" totalsRowDxfId="235">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tbl_hold_a" displayName="tbl_hold_a" ref="B124:S135" headerRowDxfId="235" dataDxfId="234" totalsRowDxfId="233">
   <autoFilter ref="B124:S135" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B125:S135">
     <sortCondition ref="C124:C135"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Cusip" totalsRowLabel="Total" dataDxfId="234" totalsRowDxfId="233"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Issuer" dataDxfId="232" totalsRowDxfId="231"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Security Description" dataDxfId="230" totalsRowDxfId="229"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Issue Date" dataDxfId="228" totalsRowDxfId="227"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Maturity Date" dataDxfId="226" totalsRowDxfId="225"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Coupon" dataDxfId="224" totalsRowDxfId="223"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Spread" dataDxfId="222" totalsRowDxfId="221"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Current Face" dataDxfId="220" totalsRowDxfId="219" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Factor" dataDxfId="218" totalsRowDxfId="217"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Market Price" dataDxfId="216" totalsRowDxfId="215"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Market Value" dataDxfId="214" totalsRowDxfId="213" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="NRSRO" dataDxfId="212" totalsRowDxfId="211"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="NRSRO Rating" dataDxfId="210" totalsRowDxfId="209"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="WAL" dataDxfId="208" totalsRowDxfId="207"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Par Sub" dataDxfId="206" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Implied DM" dataDxfId="205" totalsRowDxfId="204"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0600-000011000000}" name="Next Payment Date" dataDxfId="203" totalsRowDxfId="202"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0600-000012000000}" name="Non-Call Date" totalsRowFunction="sum" dataDxfId="201" totalsRowDxfId="200"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Cusip" totalsRowLabel="Total" dataDxfId="232" totalsRowDxfId="231"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Issuer" dataDxfId="230" totalsRowDxfId="229"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Security Description" dataDxfId="228" totalsRowDxfId="227"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Issue Date" dataDxfId="226" totalsRowDxfId="225"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Maturity Date" dataDxfId="224" totalsRowDxfId="223"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Coupon" dataDxfId="222" totalsRowDxfId="221"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Spread" dataDxfId="220" totalsRowDxfId="219"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Current Face" dataDxfId="218" totalsRowDxfId="217" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Factor" dataDxfId="216" totalsRowDxfId="215"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Market Price" dataDxfId="214" totalsRowDxfId="213"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Market Value" dataDxfId="212" totalsRowDxfId="211" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="NRSRO" dataDxfId="210" totalsRowDxfId="209"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="NRSRO Rating" dataDxfId="208" totalsRowDxfId="207"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="WAL" dataDxfId="206" totalsRowDxfId="205"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Par Sub" dataDxfId="204" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Implied DM" dataDxfId="203" totalsRowDxfId="202"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0600-000011000000}" name="Next Payment Date" dataDxfId="201" totalsRowDxfId="200"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0600-000012000000}" name="Non-Call Date" totalsRowFunction="sum" dataDxfId="199" totalsRowDxfId="198"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tbl_hold_bbb" displayName="tbl_hold_bbb" ref="B142:S155" totalsRowShown="0" headerRowDxfId="199" dataDxfId="198">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tbl_hold_bbb" displayName="tbl_hold_bbb" ref="B142:S155" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196">
   <autoFilter ref="B142:S155" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B143:S155">
     <sortCondition ref="C142:C155"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Cusip" dataDxfId="197"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Issuer" dataDxfId="196"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Security Description" dataDxfId="195"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Issue Date" dataDxfId="194"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Maturity Date" dataDxfId="193"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Coupon" dataDxfId="192"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Spread" dataDxfId="191"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Current Face" dataDxfId="190" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Factor" dataDxfId="189"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Market Price" dataDxfId="188"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Market Value" dataDxfId="187" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="NRSRO" dataDxfId="186"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="NRSRO Rating" dataDxfId="185"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="WAL" dataDxfId="184"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Par Sub" dataDxfId="183" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Implied DM" dataDxfId="182"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Next Payment Date" dataDxfId="181"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="Non-Call Date" dataDxfId="180"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Cusip" dataDxfId="195"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Issuer" dataDxfId="194"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Security Description" dataDxfId="193"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Issue Date" dataDxfId="192"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Maturity Date" dataDxfId="191"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Coupon" dataDxfId="190"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Spread" dataDxfId="189"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Current Face" dataDxfId="188" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Factor" dataDxfId="187"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Market Price" dataDxfId="186"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Market Value" dataDxfId="185" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="NRSRO" dataDxfId="184"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="NRSRO Rating" dataDxfId="183"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="WAL" dataDxfId="182"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Par Sub" dataDxfId="181" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Implied DM" dataDxfId="180"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Next Payment Date" dataDxfId="179"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="Non-Call Date" dataDxfId="178"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tbl_hold_bb" displayName="tbl_hold_bb" ref="B162:S175" totalsRowShown="0" headerRowDxfId="179" dataDxfId="178">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tbl_hold_bb" displayName="tbl_hold_bb" ref="B162:S175" totalsRowShown="0" headerRowDxfId="177" dataDxfId="176">
   <autoFilter ref="B162:S175" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B163:S175">
     <sortCondition ref="C162:C175"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Cusip" dataDxfId="177"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Issuer" dataDxfId="176"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Security Description" dataDxfId="175"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Issue Date" dataDxfId="174"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Maturity Date" dataDxfId="173"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Coupon" dataDxfId="172"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="Spread" dataDxfId="171"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Current Face" dataDxfId="170" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="Factor" dataDxfId="169"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Market Price" dataDxfId="168"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="Market Value" dataDxfId="167" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="NRSRO" dataDxfId="166"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="NRSRO Rating" dataDxfId="165"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="WAL" dataDxfId="164"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Par Sub" dataDxfId="163" dataCellStyle="Percent"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Implied DM" dataDxfId="162"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Next Payment Date" dataDxfId="161"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="Non-Call Date" dataDxfId="160"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Cusip" dataDxfId="175"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Issuer" dataDxfId="174"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Security Description" dataDxfId="173"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Issue Date" dataDxfId="172"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Maturity Date" dataDxfId="171"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Coupon" dataDxfId="170"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="Spread" dataDxfId="169"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="Current Face" dataDxfId="168" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="Factor" dataDxfId="167"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="Market Price" dataDxfId="166"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="Market Value" dataDxfId="165" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="NRSRO" dataDxfId="164"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="NRSRO Rating" dataDxfId="163"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="WAL" dataDxfId="162"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Par Sub" dataDxfId="161" dataCellStyle="Percent"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Implied DM" dataDxfId="160"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Next Payment Date" dataDxfId="159"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="Non-Call Date" dataDxfId="158"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleEldridge2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -12428,382 +12433,382 @@
       <c r="P7" s="43"/>
     </row>
     <row r="8" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="54" t="s">
         <v>1645</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
       <c r="O8" s="43"/>
       <c r="P8" s="43"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
       <c r="O9" s="43"/>
       <c r="P9" s="43"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
       <c r="O10" s="43"/>
       <c r="P10" s="43"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
       <c r="O11" s="43"/>
       <c r="P11" s="43"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
       <c r="O12" s="43"/>
       <c r="P12" s="43"/>
     </row>
     <row r="13" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="53" t="s">
         <v>1646</v>
       </c>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
       <c r="O13" s="43"/>
       <c r="P13" s="43"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
       <c r="O14" s="43"/>
       <c r="P14" s="43"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
       <c r="O15" s="43"/>
       <c r="P15" s="43"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
       <c r="O16" s="43"/>
       <c r="P16" s="43"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
       <c r="O17" s="43"/>
       <c r="P17" s="43"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="52"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
       <c r="O18" s="43"/>
       <c r="P18" s="43"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
       <c r="O19" s="43"/>
       <c r="P19" s="43"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
       <c r="O20" s="43"/>
       <c r="P20" s="43"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
       <c r="O21" s="43"/>
       <c r="P21" s="43"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="53" t="s">
         <v>1647</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
       <c r="O22" s="43"/>
       <c r="P22" s="43"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
       <c r="O23" s="43"/>
       <c r="P23" s="43"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="52"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="53"/>
       <c r="O24" s="43"/>
       <c r="P24" s="43"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="52"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="53"/>
       <c r="O25" s="43"/>
       <c r="P25" s="43"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
       <c r="O26" s="43"/>
       <c r="P26" s="43"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
       <c r="O27" s="43"/>
       <c r="P27" s="43"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
       <c r="O28" s="43"/>
       <c r="P28" s="43"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="52"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="52"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
       <c r="O29" s="43"/>
       <c r="P29" s="43"/>
     </row>
@@ -12908,9 +12913,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:S201"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="G1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13041,11 +13046,11 @@
       <c r="E10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="46">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
         <v>5.25</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="46">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
         <v>5.2668997500000003</v>
       </c>
@@ -13097,11 +13102,11 @@
       <c r="E11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="46">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
         <v>120.497963</v>
       </c>
-      <c r="G11" s="47">
+      <c r="G11" s="46">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
         <v>120.65678206999999</v>
       </c>
@@ -13155,11 +13160,11 @@
       <c r="E12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="46">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
         <v>441.253722355609</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="46">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
         <v>441.59184833</v>
       </c>
@@ -13213,11 +13218,11 @@
       <c r="E13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="46">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
         <v>2310.075090662257</v>
       </c>
-      <c r="G13" s="47">
+      <c r="G13" s="46">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
         <v>2302.270514450001</v>
       </c>
@@ -13269,11 +13274,11 @@
       <c r="E14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="46">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
         <v>234.07858784198103</v>
       </c>
-      <c r="G14" s="47">
+      <c r="G14" s="46">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
         <v>214.66817902999995</v>
       </c>
@@ -13327,11 +13332,11 @@
       <c r="E15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="46">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
         <v>21.376474690810003</v>
       </c>
-      <c r="G15" s="47">
+      <c r="G15" s="46">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
         <v>20.7037455</v>
       </c>
@@ -13385,11 +13390,11 @@
       <c r="E16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F16" s="46">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
         <v>1.2030000000000001</v>
       </c>
-      <c r="G16" s="47">
+      <c r="G16" s="46">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
         <v>0.80212671999999996</v>
       </c>
@@ -13443,11 +13448,11 @@
       <c r="E17" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="46">
         <f>Table13[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
         <v>0</v>
       </c>
-      <c r="G17" s="47">
+      <c r="G17" s="46">
         <f>Table13[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
         <v>0</v>
       </c>
@@ -13497,11 +13502,11 @@
       <c r="E18" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="48">
+      <c r="F18" s="47">
         <f>SUBTOTAL(109,Table13[Current Face (M)])</f>
         <v>3133.7348385506571</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="47">
         <f>SUBTOTAL(109,Table13[Market Value (M)])</f>
         <v>3105.9600958500009</v>
       </c>
@@ -13815,27 +13820,27 @@
         <v>1.6303516437363025E-2</v>
       </c>
       <c r="N29" s="17" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="O29" s="46">
         <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>1</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="P29" s="46">
         <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>0.90519999999999989</v>
+        <v>9.3323762100000014</v>
       </c>
       <c r="Q29" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>5.5802140297767338E-4</v>
+        <v>5.3291043984367813E-3</v>
       </c>
       <c r="R29" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>5.1212552067880735E-4</v>
+        <v>5.2798807177604568E-3</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
@@ -13886,27 +13891,27 @@
         <v>6.9418691214731584E-2</v>
       </c>
       <c r="N30" s="17" t="s">
-        <v>1523</v>
+        <v>1651</v>
       </c>
       <c r="O30" s="46">
         <f>Table21[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
-        <v>9.5500000000000007</v>
+        <v>0</v>
       </c>
       <c r="P30" s="46">
         <f>Table21[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
-        <v>9.3323762100000014</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$10,
    SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
-        <v>5.3291043984367813E-3</v>
+        <v>0</v>
       </c>
       <c r="R30" s="20">
         <f>IFERROR(IF($C$4="All Portfolios",
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]])/$C$11,
    SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Collateral Type],Table21[[#This Row],[Collateral Type]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
-        <v>5.2798807177604568E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
@@ -14097,21 +14102,21 @@
       <c r="N33" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="O33" s="51">
+      <c r="O33" s="50">
         <f>SUBTOTAL(109,Table21[Current Face (M)])</f>
-        <v>63.417653807893998</v>
-      </c>
-      <c r="P33" s="51">
+        <v>62.417653807893998</v>
+      </c>
+      <c r="P33" s="50">
         <f>SUBTOTAL(109,Table21[Market Value (M)])</f>
-        <v>59.802369249999998</v>
+        <v>58.897169250000005</v>
       </c>
       <c r="Q33" s="16">
         <f>SUBTOTAL(109,Table21[Portfolio % CF])</f>
-        <v>3.5388408151433404E-2</v>
+        <v>3.4830386748455726E-2</v>
       </c>
       <c r="R33" s="16">
         <f>SUBTOTAL(109,Table21[Portfolio % MV])</f>
-        <v>3.3833759931487573E-2</v>
+        <v>3.3321634410808765E-2</v>
       </c>
     </row>
     <row r="34" spans="2:18" ht="15" x14ac:dyDescent="0.25">
@@ -14176,29 +14181,49 @@
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.2">
       <c r="H36" s="17" t="s">
+        <v>1650</v>
+      </c>
+      <c r="I36" s="51">
+        <f>Table20[[#This Row],[Portfolio % CF]]*$C$10/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="51">
+        <f>Table20[[#This Row],[Portfolio % MV]]*$C$11/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="52">
+        <f>IFERROR(IF($C$4="All Portfolios",
+   SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$10,
+   SUMIFS(Positions!$C$2:$C$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$10),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="52">
+        <f>IFERROR(IF($C$4="All Portfolios",
+   SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]])/$C$11,
+   SUMIFS(Positions!$D$2:$D$644,tbl_rawhold[Vintage],Table20[[#This Row],[Vintage]],Positions!$M$2:$M$644,$C$4)/$C$11),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="H37" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="I36" s="46">
+      <c r="I37" s="50">
         <f>SUBTOTAL(109,Table20[Current Face (M)])</f>
         <v>3070.3171847427634</v>
       </c>
-      <c r="J36" s="46">
+      <c r="J37" s="50">
         <f>SUBTOTAL(109,Table20[Market Value (M)])</f>
         <v>3046.1577266000004</v>
       </c>
-      <c r="K36" s="16">
+      <c r="K37" s="16">
         <f>SUBTOTAL(109,Table20[Portfolio % CF])</f>
         <v>1.713302703016617</v>
       </c>
-      <c r="L36" s="16">
+      <c r="L37" s="16">
         <f>SUBTOTAL(109,Table20[Portfolio % MV])</f>
         <v>1.7233927439292949</v>
       </c>
-    </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="I37" s="17"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.2">
       <c r="I38" s="17"/>
@@ -15430,7 +15455,7 @@
       <c r="E95" s="17"/>
       <c r="F95" s="17"/>
       <c r="G95" s="10"/>
-      <c r="H95" s="49"/>
+      <c r="H95" s="48"/>
       <c r="I95" s="17"/>
       <c r="J95" s="17"/>
     </row>
@@ -15441,7 +15466,7 @@
       <c r="E96" s="17"/>
       <c r="F96" s="17"/>
       <c r="G96" s="10"/>
-      <c r="H96" s="49"/>
+      <c r="H96" s="48"/>
       <c r="I96" s="17"/>
       <c r="J96" s="17"/>
     </row>
@@ -15470,7 +15495,7 @@
       <c r="G103" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H103" s="50" t="s">
+      <c r="H103" s="49" t="s">
         <v>116</v>
       </c>
       <c r="I103" s="34" t="s">
@@ -15497,7 +15522,7 @@
       <c r="P103" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="Q103" s="50" t="s">
+      <c r="Q103" s="49" t="s">
         <v>121</v>
       </c>
       <c r="R103" s="17" t="s">
@@ -15514,7 +15539,7 @@
       <c r="E104" s="17"/>
       <c r="F104" s="17"/>
       <c r="G104" s="22"/>
-      <c r="H104" s="50"/>
+      <c r="H104" s="49"/>
       <c r="I104" s="34"/>
       <c r="J104" s="22"/>
       <c r="K104" s="22"/>
@@ -15523,7 +15548,7 @@
       <c r="N104" s="17"/>
       <c r="O104" s="22"/>
       <c r="P104" s="16"/>
-      <c r="Q104" s="50"/>
+      <c r="Q104" s="49"/>
       <c r="R104" s="17"/>
       <c r="S104" s="17"/>
     </row>
@@ -15534,7 +15559,7 @@
       <c r="E105" s="17"/>
       <c r="F105" s="17"/>
       <c r="G105" s="22"/>
-      <c r="H105" s="50"/>
+      <c r="H105" s="49"/>
       <c r="I105" s="34"/>
       <c r="J105" s="22"/>
       <c r="K105" s="22"/>
@@ -15543,7 +15568,7 @@
       <c r="N105" s="17"/>
       <c r="O105" s="22"/>
       <c r="P105" s="16"/>
-      <c r="Q105" s="50"/>
+      <c r="Q105" s="49"/>
       <c r="R105" s="17"/>
       <c r="S105" s="17"/>
     </row>
@@ -15554,7 +15579,7 @@
       <c r="E106" s="17"/>
       <c r="F106" s="17"/>
       <c r="G106" s="22"/>
-      <c r="H106" s="50"/>
+      <c r="H106" s="49"/>
       <c r="I106" s="34"/>
       <c r="J106" s="22"/>
       <c r="K106" s="22"/>
@@ -15563,7 +15588,7 @@
       <c r="N106" s="17"/>
       <c r="O106" s="22"/>
       <c r="P106" s="16"/>
-      <c r="Q106" s="50"/>
+      <c r="Q106" s="49"/>
       <c r="R106" s="17"/>
       <c r="S106" s="17"/>
     </row>
@@ -15574,7 +15599,7 @@
       <c r="E107" s="17"/>
       <c r="F107" s="17"/>
       <c r="G107" s="22"/>
-      <c r="H107" s="50"/>
+      <c r="H107" s="49"/>
       <c r="I107" s="34"/>
       <c r="J107" s="22"/>
       <c r="K107" s="22"/>
@@ -15583,7 +15608,7 @@
       <c r="N107" s="17"/>
       <c r="O107" s="22"/>
       <c r="P107" s="16"/>
-      <c r="Q107" s="50"/>
+      <c r="Q107" s="49"/>
       <c r="R107" s="17"/>
       <c r="S107" s="17"/>
     </row>
@@ -15594,7 +15619,7 @@
       <c r="E108" s="17"/>
       <c r="F108" s="17"/>
       <c r="G108" s="22"/>
-      <c r="H108" s="50"/>
+      <c r="H108" s="49"/>
       <c r="I108" s="34"/>
       <c r="J108" s="22"/>
       <c r="K108" s="22"/>
@@ -15603,7 +15628,7 @@
       <c r="N108" s="17"/>
       <c r="O108" s="22"/>
       <c r="P108" s="16"/>
-      <c r="Q108" s="50"/>
+      <c r="Q108" s="49"/>
       <c r="R108" s="17"/>
       <c r="S108" s="17"/>
     </row>
@@ -15614,7 +15639,7 @@
       <c r="E109" s="17"/>
       <c r="F109" s="17"/>
       <c r="G109" s="22"/>
-      <c r="H109" s="50"/>
+      <c r="H109" s="49"/>
       <c r="I109" s="34"/>
       <c r="J109" s="22"/>
       <c r="K109" s="22"/>
@@ -15623,7 +15648,7 @@
       <c r="N109" s="17"/>
       <c r="O109" s="22"/>
       <c r="P109" s="16"/>
-      <c r="Q109" s="50"/>
+      <c r="Q109" s="49"/>
       <c r="R109" s="17"/>
       <c r="S109" s="17"/>
     </row>
@@ -15634,7 +15659,7 @@
       <c r="E110" s="17"/>
       <c r="F110" s="17"/>
       <c r="G110" s="22"/>
-      <c r="H110" s="50"/>
+      <c r="H110" s="49"/>
       <c r="I110" s="34"/>
       <c r="J110" s="22"/>
       <c r="K110" s="22"/>
@@ -15643,7 +15668,7 @@
       <c r="N110" s="17"/>
       <c r="O110" s="22"/>
       <c r="P110" s="16"/>
-      <c r="Q110" s="50"/>
+      <c r="Q110" s="49"/>
       <c r="R110" s="17"/>
       <c r="S110" s="17"/>
     </row>
@@ -15666,7 +15691,7 @@
       <c r="G111" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H111" s="50" t="s">
+      <c r="H111" s="49" t="s">
         <v>116</v>
       </c>
       <c r="I111" s="34" t="s">
@@ -15693,7 +15718,7 @@
       <c r="P111" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="Q111" s="50" t="s">
+      <c r="Q111" s="49" t="s">
         <v>121</v>
       </c>
       <c r="R111" s="17" t="s">
@@ -15710,7 +15735,7 @@
       <c r="E112" s="17"/>
       <c r="F112" s="17"/>
       <c r="G112" s="22"/>
-      <c r="H112" s="50"/>
+      <c r="H112" s="49"/>
       <c r="I112" s="34"/>
       <c r="J112" s="22"/>
       <c r="K112" s="22"/>
@@ -15719,7 +15744,7 @@
       <c r="N112" s="17"/>
       <c r="O112" s="22"/>
       <c r="P112" s="16"/>
-      <c r="Q112" s="50"/>
+      <c r="Q112" s="49"/>
       <c r="R112" s="17"/>
       <c r="S112" s="17"/>
     </row>
@@ -15730,7 +15755,7 @@
       <c r="E113" s="17"/>
       <c r="F113" s="17"/>
       <c r="G113" s="22"/>
-      <c r="H113" s="50"/>
+      <c r="H113" s="49"/>
       <c r="I113" s="34"/>
       <c r="J113" s="22"/>
       <c r="K113" s="22"/>
@@ -15739,7 +15764,7 @@
       <c r="N113" s="17"/>
       <c r="O113" s="22"/>
       <c r="P113" s="16"/>
-      <c r="Q113" s="50"/>
+      <c r="Q113" s="49"/>
       <c r="R113" s="17"/>
       <c r="S113" s="17"/>
     </row>
@@ -15750,7 +15775,7 @@
       <c r="E114" s="17"/>
       <c r="F114" s="17"/>
       <c r="G114" s="22"/>
-      <c r="H114" s="50"/>
+      <c r="H114" s="49"/>
       <c r="I114" s="34"/>
       <c r="J114" s="22"/>
       <c r="K114" s="22"/>
@@ -15759,7 +15784,7 @@
       <c r="N114" s="17"/>
       <c r="O114" s="22"/>
       <c r="P114" s="16"/>
-      <c r="Q114" s="50"/>
+      <c r="Q114" s="49"/>
       <c r="R114" s="17"/>
       <c r="S114" s="17"/>
     </row>
@@ -15770,7 +15795,7 @@
       <c r="E115" s="17"/>
       <c r="F115" s="17"/>
       <c r="G115" s="22"/>
-      <c r="H115" s="50"/>
+      <c r="H115" s="49"/>
       <c r="I115" s="34"/>
       <c r="J115" s="22"/>
       <c r="K115" s="22"/>
@@ -15779,7 +15804,7 @@
       <c r="N115" s="17"/>
       <c r="O115" s="22"/>
       <c r="P115" s="16"/>
-      <c r="Q115" s="50"/>
+      <c r="Q115" s="49"/>
       <c r="R115" s="17"/>
       <c r="S115" s="17"/>
     </row>
@@ -15790,7 +15815,7 @@
       <c r="E116" s="17"/>
       <c r="F116" s="17"/>
       <c r="G116" s="22"/>
-      <c r="H116" s="50"/>
+      <c r="H116" s="49"/>
       <c r="I116" s="34"/>
       <c r="J116" s="22"/>
       <c r="K116" s="22"/>
@@ -15799,7 +15824,7 @@
       <c r="N116" s="17"/>
       <c r="O116" s="22"/>
       <c r="P116" s="16"/>
-      <c r="Q116" s="50"/>
+      <c r="Q116" s="49"/>
       <c r="R116" s="17"/>
       <c r="S116" s="17"/>
     </row>
@@ -15810,7 +15835,7 @@
       <c r="E117" s="17"/>
       <c r="F117" s="17"/>
       <c r="G117" s="22"/>
-      <c r="H117" s="50"/>
+      <c r="H117" s="49"/>
       <c r="I117" s="34"/>
       <c r="J117" s="22"/>
       <c r="K117" s="22"/>
@@ -15819,7 +15844,7 @@
       <c r="N117" s="17"/>
       <c r="O117" s="22"/>
       <c r="P117" s="16"/>
-      <c r="Q117" s="50"/>
+      <c r="Q117" s="49"/>
       <c r="R117" s="17"/>
       <c r="S117" s="17"/>
     </row>
@@ -15830,7 +15855,7 @@
       <c r="E118" s="17"/>
       <c r="F118" s="17"/>
       <c r="G118" s="22"/>
-      <c r="H118" s="50"/>
+      <c r="H118" s="49"/>
       <c r="I118" s="34"/>
       <c r="J118" s="22"/>
       <c r="K118" s="22"/>
@@ -15839,7 +15864,7 @@
       <c r="N118" s="17"/>
       <c r="O118" s="22"/>
       <c r="P118" s="16"/>
-      <c r="Q118" s="50"/>
+      <c r="Q118" s="49"/>
       <c r="R118" s="17"/>
       <c r="S118" s="17"/>
     </row>
@@ -15850,7 +15875,7 @@
       <c r="E119" s="17"/>
       <c r="F119" s="17"/>
       <c r="G119" s="22"/>
-      <c r="H119" s="50"/>
+      <c r="H119" s="49"/>
       <c r="I119" s="34"/>
       <c r="J119" s="22"/>
       <c r="K119" s="22"/>
@@ -15859,7 +15884,7 @@
       <c r="N119" s="17"/>
       <c r="O119" s="22"/>
       <c r="P119" s="16"/>
-      <c r="Q119" s="50"/>
+      <c r="Q119" s="49"/>
       <c r="R119" s="17"/>
       <c r="S119" s="17"/>
     </row>
@@ -15870,7 +15895,7 @@
       <c r="E120" s="17"/>
       <c r="F120" s="17"/>
       <c r="G120" s="22"/>
-      <c r="H120" s="50"/>
+      <c r="H120" s="49"/>
       <c r="I120" s="34"/>
       <c r="J120" s="22"/>
       <c r="K120" s="22"/>
@@ -15879,7 +15904,7 @@
       <c r="N120" s="17"/>
       <c r="O120" s="22"/>
       <c r="P120" s="16"/>
-      <c r="Q120" s="50"/>
+      <c r="Q120" s="49"/>
       <c r="R120" s="17"/>
       <c r="S120" s="17"/>
     </row>
@@ -15890,7 +15915,7 @@
       <c r="E121" s="17"/>
       <c r="F121" s="17"/>
       <c r="G121" s="22"/>
-      <c r="H121" s="50"/>
+      <c r="H121" s="49"/>
       <c r="I121" s="34"/>
       <c r="J121" s="22"/>
       <c r="K121" s="22"/>
@@ -15899,7 +15924,7 @@
       <c r="N121" s="17"/>
       <c r="O121" s="22"/>
       <c r="P121" s="16"/>
-      <c r="Q121" s="50"/>
+      <c r="Q121" s="49"/>
       <c r="R121" s="17"/>
       <c r="S121" s="17"/>
     </row>
@@ -15910,7 +15935,7 @@
       <c r="E122" s="17"/>
       <c r="F122" s="17"/>
       <c r="G122" s="22"/>
-      <c r="H122" s="50"/>
+      <c r="H122" s="49"/>
       <c r="I122" s="34"/>
       <c r="J122" s="22"/>
       <c r="K122" s="22"/>
@@ -15919,7 +15944,7 @@
       <c r="N122" s="17"/>
       <c r="O122" s="22"/>
       <c r="P122" s="16"/>
-      <c r="Q122" s="50"/>
+      <c r="Q122" s="49"/>
       <c r="R122" s="17"/>
       <c r="S122" s="17"/>
     </row>
@@ -15930,7 +15955,7 @@
       <c r="E123" s="17"/>
       <c r="F123" s="17"/>
       <c r="G123" s="22"/>
-      <c r="H123" s="50"/>
+      <c r="H123" s="49"/>
       <c r="I123" s="34"/>
       <c r="J123" s="22"/>
       <c r="K123" s="22"/>
@@ -15939,7 +15964,7 @@
       <c r="N123" s="17"/>
       <c r="O123" s="22"/>
       <c r="P123" s="16"/>
-      <c r="Q123" s="50"/>
+      <c r="Q123" s="49"/>
       <c r="R123" s="17"/>
       <c r="S123" s="17"/>
     </row>
@@ -15962,7 +15987,7 @@
       <c r="G124" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H124" s="50" t="s">
+      <c r="H124" s="49" t="s">
         <v>116</v>
       </c>
       <c r="I124" s="34" t="s">
@@ -15989,7 +16014,7 @@
       <c r="P124" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="Q124" s="50" t="s">
+      <c r="Q124" s="49" t="s">
         <v>121</v>
       </c>
       <c r="R124" s="17" t="s">
@@ -16006,7 +16031,7 @@
       <c r="E125" s="17"/>
       <c r="F125" s="17"/>
       <c r="G125" s="22"/>
-      <c r="H125" s="50"/>
+      <c r="H125" s="49"/>
       <c r="I125" s="34"/>
       <c r="J125" s="22"/>
       <c r="K125" s="22"/>
@@ -16015,7 +16040,7 @@
       <c r="N125" s="17"/>
       <c r="O125" s="22"/>
       <c r="P125" s="16"/>
-      <c r="Q125" s="50"/>
+      <c r="Q125" s="49"/>
       <c r="R125" s="17"/>
       <c r="S125" s="17"/>
     </row>
@@ -16026,7 +16051,7 @@
       <c r="E126" s="17"/>
       <c r="F126" s="17"/>
       <c r="G126" s="22"/>
-      <c r="H126" s="50"/>
+      <c r="H126" s="49"/>
       <c r="I126" s="34"/>
       <c r="J126" s="22"/>
       <c r="K126" s="22"/>
@@ -16035,7 +16060,7 @@
       <c r="N126" s="17"/>
       <c r="O126" s="22"/>
       <c r="P126" s="16"/>
-      <c r="Q126" s="50"/>
+      <c r="Q126" s="49"/>
       <c r="R126" s="17"/>
       <c r="S126" s="17"/>
     </row>
@@ -16046,7 +16071,7 @@
       <c r="E127" s="17"/>
       <c r="F127" s="17"/>
       <c r="G127" s="22"/>
-      <c r="H127" s="50"/>
+      <c r="H127" s="49"/>
       <c r="I127" s="34"/>
       <c r="J127" s="22"/>
       <c r="K127" s="22"/>
@@ -16055,7 +16080,7 @@
       <c r="N127" s="17"/>
       <c r="O127" s="22"/>
       <c r="P127" s="16"/>
-      <c r="Q127" s="50"/>
+      <c r="Q127" s="49"/>
       <c r="R127" s="17"/>
       <c r="S127" s="17"/>
     </row>
@@ -16066,7 +16091,7 @@
       <c r="E128" s="17"/>
       <c r="F128" s="17"/>
       <c r="G128" s="22"/>
-      <c r="H128" s="50"/>
+      <c r="H128" s="49"/>
       <c r="I128" s="34"/>
       <c r="J128" s="22"/>
       <c r="K128" s="22"/>
@@ -16075,7 +16100,7 @@
       <c r="N128" s="17"/>
       <c r="O128" s="22"/>
       <c r="P128" s="16"/>
-      <c r="Q128" s="50"/>
+      <c r="Q128" s="49"/>
       <c r="R128" s="17"/>
       <c r="S128" s="17"/>
     </row>
@@ -16086,7 +16111,7 @@
       <c r="E129" s="17"/>
       <c r="F129" s="17"/>
       <c r="G129" s="22"/>
-      <c r="H129" s="50"/>
+      <c r="H129" s="49"/>
       <c r="I129" s="34"/>
       <c r="J129" s="22"/>
       <c r="K129" s="22"/>
@@ -16095,7 +16120,7 @@
       <c r="N129" s="17"/>
       <c r="O129" s="22"/>
       <c r="P129" s="16"/>
-      <c r="Q129" s="50"/>
+      <c r="Q129" s="49"/>
       <c r="R129" s="17"/>
       <c r="S129" s="17"/>
     </row>
@@ -16106,7 +16131,7 @@
       <c r="E130" s="17"/>
       <c r="F130" s="17"/>
       <c r="G130" s="22"/>
-      <c r="H130" s="50"/>
+      <c r="H130" s="49"/>
       <c r="I130" s="34"/>
       <c r="J130" s="22"/>
       <c r="K130" s="22"/>
@@ -16115,7 +16140,7 @@
       <c r="N130" s="17"/>
       <c r="O130" s="22"/>
       <c r="P130" s="16"/>
-      <c r="Q130" s="50"/>
+      <c r="Q130" s="49"/>
       <c r="R130" s="17"/>
       <c r="S130" s="17"/>
     </row>
@@ -16126,7 +16151,7 @@
       <c r="E131" s="17"/>
       <c r="F131" s="17"/>
       <c r="G131" s="22"/>
-      <c r="H131" s="50"/>
+      <c r="H131" s="49"/>
       <c r="I131" s="34"/>
       <c r="J131" s="22"/>
       <c r="K131" s="22"/>
@@ -16135,7 +16160,7 @@
       <c r="N131" s="17"/>
       <c r="O131" s="22"/>
       <c r="P131" s="16"/>
-      <c r="Q131" s="50"/>
+      <c r="Q131" s="49"/>
       <c r="R131" s="17"/>
       <c r="S131" s="17"/>
     </row>
@@ -16146,7 +16171,7 @@
       <c r="E132" s="17"/>
       <c r="F132" s="17"/>
       <c r="G132" s="22"/>
-      <c r="H132" s="50"/>
+      <c r="H132" s="49"/>
       <c r="I132" s="34"/>
       <c r="J132" s="22"/>
       <c r="K132" s="22"/>
@@ -16155,7 +16180,7 @@
       <c r="N132" s="17"/>
       <c r="O132" s="22"/>
       <c r="P132" s="16"/>
-      <c r="Q132" s="50"/>
+      <c r="Q132" s="49"/>
       <c r="R132" s="17"/>
       <c r="S132" s="17"/>
     </row>
@@ -16166,7 +16191,7 @@
       <c r="E133" s="17"/>
       <c r="F133" s="17"/>
       <c r="G133" s="22"/>
-      <c r="H133" s="50"/>
+      <c r="H133" s="49"/>
       <c r="I133" s="34"/>
       <c r="J133" s="22"/>
       <c r="K133" s="22"/>
@@ -16175,7 +16200,7 @@
       <c r="N133" s="17"/>
       <c r="O133" s="22"/>
       <c r="P133" s="16"/>
-      <c r="Q133" s="50"/>
+      <c r="Q133" s="49"/>
       <c r="R133" s="17"/>
       <c r="S133" s="17"/>
     </row>
@@ -16186,7 +16211,7 @@
       <c r="E134" s="17"/>
       <c r="F134" s="17"/>
       <c r="G134" s="22"/>
-      <c r="H134" s="50"/>
+      <c r="H134" s="49"/>
       <c r="I134" s="34"/>
       <c r="J134" s="22"/>
       <c r="K134" s="22"/>
@@ -16195,7 +16220,7 @@
       <c r="N134" s="17"/>
       <c r="O134" s="22"/>
       <c r="P134" s="16"/>
-      <c r="Q134" s="50"/>
+      <c r="Q134" s="49"/>
       <c r="R134" s="17"/>
       <c r="S134" s="17"/>
     </row>
@@ -16206,7 +16231,7 @@
       <c r="E135" s="17"/>
       <c r="F135" s="17"/>
       <c r="G135" s="22"/>
-      <c r="H135" s="50"/>
+      <c r="H135" s="49"/>
       <c r="I135" s="34"/>
       <c r="J135" s="22"/>
       <c r="K135" s="22"/>
@@ -16215,7 +16240,7 @@
       <c r="N135" s="17"/>
       <c r="O135" s="22"/>
       <c r="P135" s="16"/>
-      <c r="Q135" s="50"/>
+      <c r="Q135" s="49"/>
       <c r="R135" s="17"/>
       <c r="S135" s="17"/>
     </row>
@@ -16226,7 +16251,7 @@
       <c r="E136" s="17"/>
       <c r="F136" s="17"/>
       <c r="G136" s="22"/>
-      <c r="H136" s="50"/>
+      <c r="H136" s="49"/>
       <c r="I136" s="34"/>
       <c r="J136" s="22"/>
       <c r="K136" s="22"/>
@@ -16235,7 +16260,7 @@
       <c r="N136" s="17"/>
       <c r="O136" s="22"/>
       <c r="P136" s="16"/>
-      <c r="Q136" s="50"/>
+      <c r="Q136" s="49"/>
       <c r="R136" s="17"/>
       <c r="S136" s="17"/>
     </row>
@@ -16246,7 +16271,7 @@
       <c r="E137" s="17"/>
       <c r="F137" s="17"/>
       <c r="G137" s="22"/>
-      <c r="H137" s="50"/>
+      <c r="H137" s="49"/>
       <c r="I137" s="34"/>
       <c r="J137" s="22"/>
       <c r="K137" s="22"/>
@@ -16255,7 +16280,7 @@
       <c r="N137" s="17"/>
       <c r="O137" s="22"/>
       <c r="P137" s="16"/>
-      <c r="Q137" s="50"/>
+      <c r="Q137" s="49"/>
       <c r="R137" s="17"/>
       <c r="S137" s="17"/>
     </row>
@@ -16266,7 +16291,7 @@
       <c r="E138" s="17"/>
       <c r="F138" s="17"/>
       <c r="G138" s="22"/>
-      <c r="H138" s="50"/>
+      <c r="H138" s="49"/>
       <c r="I138" s="34"/>
       <c r="J138" s="22"/>
       <c r="K138" s="22"/>
@@ -16275,7 +16300,7 @@
       <c r="N138" s="17"/>
       <c r="O138" s="22"/>
       <c r="P138" s="16"/>
-      <c r="Q138" s="50"/>
+      <c r="Q138" s="49"/>
       <c r="R138" s="17"/>
       <c r="S138" s="17"/>
     </row>
@@ -16286,7 +16311,7 @@
       <c r="E139" s="17"/>
       <c r="F139" s="17"/>
       <c r="G139" s="22"/>
-      <c r="H139" s="50"/>
+      <c r="H139" s="49"/>
       <c r="I139" s="34"/>
       <c r="J139" s="22"/>
       <c r="K139" s="22"/>
@@ -16295,7 +16320,7 @@
       <c r="N139" s="17"/>
       <c r="O139" s="22"/>
       <c r="P139" s="16"/>
-      <c r="Q139" s="50"/>
+      <c r="Q139" s="49"/>
       <c r="R139" s="17"/>
       <c r="S139" s="17"/>
     </row>
@@ -16306,7 +16331,7 @@
       <c r="E140" s="17"/>
       <c r="F140" s="17"/>
       <c r="G140" s="22"/>
-      <c r="H140" s="50"/>
+      <c r="H140" s="49"/>
       <c r="I140" s="34"/>
       <c r="J140" s="22"/>
       <c r="K140" s="22"/>
@@ -16315,7 +16340,7 @@
       <c r="N140" s="17"/>
       <c r="O140" s="22"/>
       <c r="P140" s="16"/>
-      <c r="Q140" s="50"/>
+      <c r="Q140" s="49"/>
       <c r="R140" s="17"/>
       <c r="S140" s="17"/>
     </row>
@@ -16326,7 +16351,7 @@
       <c r="E141" s="17"/>
       <c r="F141" s="17"/>
       <c r="G141" s="22"/>
-      <c r="H141" s="50"/>
+      <c r="H141" s="49"/>
       <c r="I141" s="34"/>
       <c r="J141" s="22"/>
       <c r="K141" s="22"/>
@@ -16335,7 +16360,7 @@
       <c r="N141" s="17"/>
       <c r="O141" s="22"/>
       <c r="P141" s="16"/>
-      <c r="Q141" s="50"/>
+      <c r="Q141" s="49"/>
       <c r="R141" s="17"/>
       <c r="S141" s="17"/>
     </row>
@@ -16358,7 +16383,7 @@
       <c r="G142" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H142" s="50" t="s">
+      <c r="H142" s="49" t="s">
         <v>116</v>
       </c>
       <c r="I142" s="34" t="s">
@@ -16385,7 +16410,7 @@
       <c r="P142" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="Q142" s="50" t="s">
+      <c r="Q142" s="49" t="s">
         <v>121</v>
       </c>
       <c r="R142" s="17" t="s">
@@ -16402,7 +16427,7 @@
       <c r="E143" s="17"/>
       <c r="F143" s="17"/>
       <c r="G143" s="22"/>
-      <c r="H143" s="50"/>
+      <c r="H143" s="49"/>
       <c r="I143" s="34"/>
       <c r="J143" s="22"/>
       <c r="K143" s="22"/>
@@ -16411,7 +16436,7 @@
       <c r="N143" s="17"/>
       <c r="O143" s="22"/>
       <c r="P143" s="16"/>
-      <c r="Q143" s="50"/>
+      <c r="Q143" s="49"/>
       <c r="R143" s="17"/>
       <c r="S143" s="17"/>
     </row>
@@ -16422,7 +16447,7 @@
       <c r="E144" s="17"/>
       <c r="F144" s="17"/>
       <c r="G144" s="22"/>
-      <c r="H144" s="50"/>
+      <c r="H144" s="49"/>
       <c r="I144" s="34"/>
       <c r="J144" s="22"/>
       <c r="K144" s="22"/>
@@ -16431,7 +16456,7 @@
       <c r="N144" s="17"/>
       <c r="O144" s="22"/>
       <c r="P144" s="16"/>
-      <c r="Q144" s="50"/>
+      <c r="Q144" s="49"/>
       <c r="R144" s="17"/>
       <c r="S144" s="17"/>
     </row>
@@ -16442,7 +16467,7 @@
       <c r="E145" s="17"/>
       <c r="F145" s="17"/>
       <c r="G145" s="22"/>
-      <c r="H145" s="50"/>
+      <c r="H145" s="49"/>
       <c r="I145" s="34"/>
       <c r="J145" s="22"/>
       <c r="K145" s="22"/>
@@ -16451,7 +16476,7 @@
       <c r="N145" s="17"/>
       <c r="O145" s="22"/>
       <c r="P145" s="16"/>
-      <c r="Q145" s="50"/>
+      <c r="Q145" s="49"/>
       <c r="R145" s="17"/>
       <c r="S145" s="17"/>
     </row>
@@ -16462,7 +16487,7 @@
       <c r="E146" s="17"/>
       <c r="F146" s="17"/>
       <c r="G146" s="22"/>
-      <c r="H146" s="50"/>
+      <c r="H146" s="49"/>
       <c r="I146" s="34"/>
       <c r="J146" s="22"/>
       <c r="K146" s="22"/>
@@ -16471,7 +16496,7 @@
       <c r="N146" s="17"/>
       <c r="O146" s="22"/>
       <c r="P146" s="16"/>
-      <c r="Q146" s="50"/>
+      <c r="Q146" s="49"/>
       <c r="R146" s="17"/>
       <c r="S146" s="17"/>
     </row>
@@ -16482,7 +16507,7 @@
       <c r="E147" s="17"/>
       <c r="F147" s="17"/>
       <c r="G147" s="22"/>
-      <c r="H147" s="50"/>
+      <c r="H147" s="49"/>
       <c r="I147" s="34"/>
       <c r="J147" s="22"/>
       <c r="K147" s="22"/>
@@ -16491,7 +16516,7 @@
       <c r="N147" s="17"/>
       <c r="O147" s="22"/>
       <c r="P147" s="16"/>
-      <c r="Q147" s="50"/>
+      <c r="Q147" s="49"/>
       <c r="R147" s="17"/>
       <c r="S147" s="17"/>
     </row>
@@ -16502,7 +16527,7 @@
       <c r="E148" s="17"/>
       <c r="F148" s="17"/>
       <c r="G148" s="22"/>
-      <c r="H148" s="50"/>
+      <c r="H148" s="49"/>
       <c r="I148" s="34"/>
       <c r="J148" s="22"/>
       <c r="K148" s="22"/>
@@ -16511,7 +16536,7 @@
       <c r="N148" s="17"/>
       <c r="O148" s="22"/>
       <c r="P148" s="16"/>
-      <c r="Q148" s="50"/>
+      <c r="Q148" s="49"/>
       <c r="R148" s="17"/>
       <c r="S148" s="17"/>
     </row>
@@ -16522,7 +16547,7 @@
       <c r="E149" s="17"/>
       <c r="F149" s="17"/>
       <c r="G149" s="22"/>
-      <c r="H149" s="50"/>
+      <c r="H149" s="49"/>
       <c r="I149" s="34"/>
       <c r="J149" s="22"/>
       <c r="K149" s="22"/>
@@ -16531,7 +16556,7 @@
       <c r="N149" s="17"/>
       <c r="O149" s="22"/>
       <c r="P149" s="16"/>
-      <c r="Q149" s="50"/>
+      <c r="Q149" s="49"/>
       <c r="R149" s="17"/>
       <c r="S149" s="17"/>
     </row>
@@ -16542,7 +16567,7 @@
       <c r="E150" s="17"/>
       <c r="F150" s="17"/>
       <c r="G150" s="22"/>
-      <c r="H150" s="50"/>
+      <c r="H150" s="49"/>
       <c r="I150" s="34"/>
       <c r="J150" s="22"/>
       <c r="K150" s="22"/>
@@ -16551,7 +16576,7 @@
       <c r="N150" s="17"/>
       <c r="O150" s="22"/>
       <c r="P150" s="16"/>
-      <c r="Q150" s="50"/>
+      <c r="Q150" s="49"/>
       <c r="R150" s="17"/>
       <c r="S150" s="17"/>
     </row>
@@ -16562,7 +16587,7 @@
       <c r="E151" s="17"/>
       <c r="F151" s="17"/>
       <c r="G151" s="22"/>
-      <c r="H151" s="50"/>
+      <c r="H151" s="49"/>
       <c r="I151" s="34"/>
       <c r="J151" s="22"/>
       <c r="K151" s="22"/>
@@ -16571,7 +16596,7 @@
       <c r="N151" s="17"/>
       <c r="O151" s="22"/>
       <c r="P151" s="16"/>
-      <c r="Q151" s="50"/>
+      <c r="Q151" s="49"/>
       <c r="R151" s="17"/>
       <c r="S151" s="17"/>
     </row>
@@ -16582,7 +16607,7 @@
       <c r="E152" s="17"/>
       <c r="F152" s="17"/>
       <c r="G152" s="22"/>
-      <c r="H152" s="50"/>
+      <c r="H152" s="49"/>
       <c r="I152" s="34"/>
       <c r="J152" s="22"/>
       <c r="K152" s="22"/>
@@ -16591,7 +16616,7 @@
       <c r="N152" s="17"/>
       <c r="O152" s="22"/>
       <c r="P152" s="16"/>
-      <c r="Q152" s="50"/>
+      <c r="Q152" s="49"/>
       <c r="R152" s="17"/>
       <c r="S152" s="17"/>
     </row>
@@ -16602,7 +16627,7 @@
       <c r="E153" s="17"/>
       <c r="F153" s="17"/>
       <c r="G153" s="22"/>
-      <c r="H153" s="50"/>
+      <c r="H153" s="49"/>
       <c r="I153" s="34"/>
       <c r="J153" s="22"/>
       <c r="K153" s="22"/>
@@ -16611,7 +16636,7 @@
       <c r="N153" s="17"/>
       <c r="O153" s="22"/>
       <c r="P153" s="16"/>
-      <c r="Q153" s="50"/>
+      <c r="Q153" s="49"/>
       <c r="R153" s="17"/>
       <c r="S153" s="17"/>
     </row>
@@ -16622,7 +16647,7 @@
       <c r="E154" s="17"/>
       <c r="F154" s="17"/>
       <c r="G154" s="22"/>
-      <c r="H154" s="50"/>
+      <c r="H154" s="49"/>
       <c r="I154" s="34"/>
       <c r="J154" s="22"/>
       <c r="K154" s="22"/>
@@ -16631,7 +16656,7 @@
       <c r="N154" s="17"/>
       <c r="O154" s="22"/>
       <c r="P154" s="16"/>
-      <c r="Q154" s="50"/>
+      <c r="Q154" s="49"/>
       <c r="R154" s="17"/>
       <c r="S154" s="17"/>
     </row>
@@ -16642,7 +16667,7 @@
       <c r="E155" s="17"/>
       <c r="F155" s="17"/>
       <c r="G155" s="22"/>
-      <c r="H155" s="50"/>
+      <c r="H155" s="49"/>
       <c r="I155" s="34"/>
       <c r="J155" s="22"/>
       <c r="K155" s="22"/>
@@ -16651,7 +16676,7 @@
       <c r="N155" s="17"/>
       <c r="O155" s="22"/>
       <c r="P155" s="16"/>
-      <c r="Q155" s="50"/>
+      <c r="Q155" s="49"/>
       <c r="R155" s="17"/>
       <c r="S155" s="17"/>
     </row>
@@ -16662,7 +16687,7 @@
       <c r="E156" s="17"/>
       <c r="F156" s="17"/>
       <c r="G156" s="22"/>
-      <c r="H156" s="50"/>
+      <c r="H156" s="49"/>
       <c r="I156" s="34"/>
       <c r="J156" s="22"/>
       <c r="K156" s="22"/>
@@ -16671,7 +16696,7 @@
       <c r="N156" s="17"/>
       <c r="O156" s="22"/>
       <c r="P156" s="16"/>
-      <c r="Q156" s="50"/>
+      <c r="Q156" s="49"/>
       <c r="R156" s="17"/>
       <c r="S156" s="17"/>
     </row>
@@ -16682,7 +16707,7 @@
       <c r="E157" s="17"/>
       <c r="F157" s="17"/>
       <c r="G157" s="22"/>
-      <c r="H157" s="50"/>
+      <c r="H157" s="49"/>
       <c r="I157" s="34"/>
       <c r="J157" s="22"/>
       <c r="K157" s="22"/>
@@ -16691,7 +16716,7 @@
       <c r="N157" s="17"/>
       <c r="O157" s="22"/>
       <c r="P157" s="16"/>
-      <c r="Q157" s="50"/>
+      <c r="Q157" s="49"/>
       <c r="R157" s="17"/>
       <c r="S157" s="17"/>
     </row>
@@ -16702,7 +16727,7 @@
       <c r="E158" s="17"/>
       <c r="F158" s="17"/>
       <c r="G158" s="22"/>
-      <c r="H158" s="50"/>
+      <c r="H158" s="49"/>
       <c r="I158" s="34"/>
       <c r="J158" s="22"/>
       <c r="K158" s="22"/>
@@ -16711,7 +16736,7 @@
       <c r="N158" s="17"/>
       <c r="O158" s="22"/>
       <c r="P158" s="16"/>
-      <c r="Q158" s="50"/>
+      <c r="Q158" s="49"/>
       <c r="R158" s="17"/>
       <c r="S158" s="17"/>
     </row>
@@ -16722,7 +16747,7 @@
       <c r="E159" s="17"/>
       <c r="F159" s="17"/>
       <c r="G159" s="22"/>
-      <c r="H159" s="50"/>
+      <c r="H159" s="49"/>
       <c r="I159" s="34"/>
       <c r="J159" s="22"/>
       <c r="K159" s="22"/>
@@ -16731,7 +16756,7 @@
       <c r="N159" s="17"/>
       <c r="O159" s="22"/>
       <c r="P159" s="16"/>
-      <c r="Q159" s="50"/>
+      <c r="Q159" s="49"/>
       <c r="R159" s="17"/>
       <c r="S159" s="17"/>
     </row>
@@ -16742,7 +16767,7 @@
       <c r="E160" s="17"/>
       <c r="F160" s="17"/>
       <c r="G160" s="22"/>
-      <c r="H160" s="50"/>
+      <c r="H160" s="49"/>
       <c r="I160" s="34"/>
       <c r="J160" s="22"/>
       <c r="K160" s="22"/>
@@ -16751,7 +16776,7 @@
       <c r="N160" s="17"/>
       <c r="O160" s="22"/>
       <c r="P160" s="16"/>
-      <c r="Q160" s="50"/>
+      <c r="Q160" s="49"/>
       <c r="R160" s="17"/>
       <c r="S160" s="17"/>
     </row>
@@ -16762,7 +16787,7 @@
       <c r="E161" s="17"/>
       <c r="F161" s="17"/>
       <c r="G161" s="22"/>
-      <c r="H161" s="50"/>
+      <c r="H161" s="49"/>
       <c r="I161" s="34"/>
       <c r="J161" s="22"/>
       <c r="K161" s="22"/>
@@ -16771,7 +16796,7 @@
       <c r="N161" s="17"/>
       <c r="O161" s="22"/>
       <c r="P161" s="16"/>
-      <c r="Q161" s="50"/>
+      <c r="Q161" s="49"/>
       <c r="R161" s="17"/>
       <c r="S161" s="17"/>
     </row>
@@ -16794,7 +16819,7 @@
       <c r="G162" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H162" s="50" t="s">
+      <c r="H162" s="49" t="s">
         <v>116</v>
       </c>
       <c r="I162" s="34" t="s">
@@ -16821,7 +16846,7 @@
       <c r="P162" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="Q162" s="50" t="s">
+      <c r="Q162" s="49" t="s">
         <v>121</v>
       </c>
       <c r="R162" s="17" t="s">
@@ -16838,7 +16863,7 @@
       <c r="E163" s="17"/>
       <c r="F163" s="17"/>
       <c r="G163" s="22"/>
-      <c r="H163" s="50"/>
+      <c r="H163" s="49"/>
       <c r="I163" s="34"/>
       <c r="J163" s="22"/>
       <c r="K163" s="22"/>
@@ -16847,7 +16872,7 @@
       <c r="N163" s="17"/>
       <c r="O163" s="22"/>
       <c r="P163" s="16"/>
-      <c r="Q163" s="50"/>
+      <c r="Q163" s="49"/>
       <c r="R163" s="17"/>
       <c r="S163" s="17"/>
     </row>
@@ -16858,7 +16883,7 @@
       <c r="E164" s="17"/>
       <c r="F164" s="17"/>
       <c r="G164" s="22"/>
-      <c r="H164" s="50"/>
+      <c r="H164" s="49"/>
       <c r="I164" s="34"/>
       <c r="J164" s="22"/>
       <c r="K164" s="22"/>
@@ -16867,7 +16892,7 @@
       <c r="N164" s="17"/>
       <c r="O164" s="22"/>
       <c r="P164" s="16"/>
-      <c r="Q164" s="50"/>
+      <c r="Q164" s="49"/>
       <c r="R164" s="17"/>
       <c r="S164" s="17"/>
     </row>
@@ -16878,7 +16903,7 @@
       <c r="E165" s="17"/>
       <c r="F165" s="17"/>
       <c r="G165" s="22"/>
-      <c r="H165" s="50"/>
+      <c r="H165" s="49"/>
       <c r="I165" s="34"/>
       <c r="J165" s="22"/>
       <c r="K165" s="22"/>
@@ -16887,7 +16912,7 @@
       <c r="N165" s="17"/>
       <c r="O165" s="22"/>
       <c r="P165" s="16"/>
-      <c r="Q165" s="50"/>
+      <c r="Q165" s="49"/>
       <c r="R165" s="17"/>
       <c r="S165" s="17"/>
     </row>
@@ -16898,7 +16923,7 @@
       <c r="E166" s="17"/>
       <c r="F166" s="17"/>
       <c r="G166" s="22"/>
-      <c r="H166" s="50"/>
+      <c r="H166" s="49"/>
       <c r="I166" s="34"/>
       <c r="J166" s="22"/>
       <c r="K166" s="22"/>
@@ -16907,7 +16932,7 @@
       <c r="N166" s="17"/>
       <c r="O166" s="22"/>
       <c r="P166" s="16"/>
-      <c r="Q166" s="50"/>
+      <c r="Q166" s="49"/>
       <c r="R166" s="17"/>
       <c r="S166" s="17"/>
     </row>
@@ -16918,7 +16943,7 @@
       <c r="E167" s="17"/>
       <c r="F167" s="17"/>
       <c r="G167" s="22"/>
-      <c r="H167" s="50"/>
+      <c r="H167" s="49"/>
       <c r="I167" s="34"/>
       <c r="J167" s="22"/>
       <c r="K167" s="22"/>
@@ -16927,7 +16952,7 @@
       <c r="N167" s="17"/>
       <c r="O167" s="22"/>
       <c r="P167" s="16"/>
-      <c r="Q167" s="50"/>
+      <c r="Q167" s="49"/>
       <c r="R167" s="17"/>
       <c r="S167" s="17"/>
     </row>
@@ -16938,7 +16963,7 @@
       <c r="E168" s="17"/>
       <c r="F168" s="17"/>
       <c r="G168" s="22"/>
-      <c r="H168" s="50"/>
+      <c r="H168" s="49"/>
       <c r="I168" s="34"/>
       <c r="J168" s="22"/>
       <c r="K168" s="22"/>
@@ -16947,7 +16972,7 @@
       <c r="N168" s="17"/>
       <c r="O168" s="22"/>
       <c r="P168" s="16"/>
-      <c r="Q168" s="50"/>
+      <c r="Q168" s="49"/>
       <c r="R168" s="17"/>
       <c r="S168" s="17"/>
     </row>
@@ -16958,7 +16983,7 @@
       <c r="E169" s="17"/>
       <c r="F169" s="17"/>
       <c r="G169" s="22"/>
-      <c r="H169" s="50"/>
+      <c r="H169" s="49"/>
       <c r="I169" s="34"/>
       <c r="J169" s="22"/>
       <c r="K169" s="22"/>
@@ -16967,7 +16992,7 @@
       <c r="N169" s="17"/>
       <c r="O169" s="22"/>
       <c r="P169" s="16"/>
-      <c r="Q169" s="50"/>
+      <c r="Q169" s="49"/>
       <c r="R169" s="17"/>
       <c r="S169" s="17"/>
     </row>
@@ -16978,7 +17003,7 @@
       <c r="E170" s="17"/>
       <c r="F170" s="17"/>
       <c r="G170" s="22"/>
-      <c r="H170" s="50"/>
+      <c r="H170" s="49"/>
       <c r="I170" s="34"/>
       <c r="J170" s="22"/>
       <c r="K170" s="22"/>
@@ -16987,7 +17012,7 @@
       <c r="N170" s="17"/>
       <c r="O170" s="22"/>
       <c r="P170" s="16"/>
-      <c r="Q170" s="50"/>
+      <c r="Q170" s="49"/>
       <c r="R170" s="17"/>
       <c r="S170" s="17"/>
     </row>
@@ -16998,7 +17023,7 @@
       <c r="E171" s="17"/>
       <c r="F171" s="17"/>
       <c r="G171" s="22"/>
-      <c r="H171" s="50"/>
+      <c r="H171" s="49"/>
       <c r="I171" s="34"/>
       <c r="J171" s="22"/>
       <c r="K171" s="22"/>
@@ -17007,7 +17032,7 @@
       <c r="N171" s="17"/>
       <c r="O171" s="22"/>
       <c r="P171" s="16"/>
-      <c r="Q171" s="50"/>
+      <c r="Q171" s="49"/>
       <c r="R171" s="17"/>
       <c r="S171" s="17"/>
     </row>
@@ -17018,7 +17043,7 @@
       <c r="E172" s="17"/>
       <c r="F172" s="17"/>
       <c r="G172" s="22"/>
-      <c r="H172" s="50"/>
+      <c r="H172" s="49"/>
       <c r="I172" s="34"/>
       <c r="J172" s="22"/>
       <c r="K172" s="22"/>
@@ -17027,7 +17052,7 @@
       <c r="N172" s="17"/>
       <c r="O172" s="22"/>
       <c r="P172" s="16"/>
-      <c r="Q172" s="50"/>
+      <c r="Q172" s="49"/>
       <c r="R172" s="17"/>
       <c r="S172" s="17"/>
     </row>
@@ -17038,7 +17063,7 @@
       <c r="E173" s="17"/>
       <c r="F173" s="17"/>
       <c r="G173" s="22"/>
-      <c r="H173" s="50"/>
+      <c r="H173" s="49"/>
       <c r="I173" s="34"/>
       <c r="J173" s="22"/>
       <c r="K173" s="22"/>
@@ -17047,7 +17072,7 @@
       <c r="N173" s="17"/>
       <c r="O173" s="22"/>
       <c r="P173" s="16"/>
-      <c r="Q173" s="50"/>
+      <c r="Q173" s="49"/>
       <c r="R173" s="17"/>
       <c r="S173" s="17"/>
     </row>
@@ -17058,7 +17083,7 @@
       <c r="E174" s="17"/>
       <c r="F174" s="17"/>
       <c r="G174" s="22"/>
-      <c r="H174" s="50"/>
+      <c r="H174" s="49"/>
       <c r="I174" s="34"/>
       <c r="J174" s="22"/>
       <c r="K174" s="22"/>
@@ -17067,7 +17092,7 @@
       <c r="N174" s="17"/>
       <c r="O174" s="22"/>
       <c r="P174" s="16"/>
-      <c r="Q174" s="50"/>
+      <c r="Q174" s="49"/>
       <c r="R174" s="17"/>
       <c r="S174" s="17"/>
     </row>
@@ -17078,7 +17103,7 @@
       <c r="E175" s="17"/>
       <c r="F175" s="17"/>
       <c r="G175" s="22"/>
-      <c r="H175" s="50"/>
+      <c r="H175" s="49"/>
       <c r="I175" s="34"/>
       <c r="J175" s="22"/>
       <c r="K175" s="22"/>
@@ -17087,7 +17112,7 @@
       <c r="N175" s="17"/>
       <c r="O175" s="22"/>
       <c r="P175" s="16"/>
-      <c r="Q175" s="50"/>
+      <c r="Q175" s="49"/>
       <c r="R175" s="17"/>
       <c r="S175" s="17"/>
     </row>
@@ -17098,7 +17123,7 @@
       <c r="E176" s="17"/>
       <c r="F176" s="17"/>
       <c r="G176" s="22"/>
-      <c r="H176" s="50"/>
+      <c r="H176" s="49"/>
       <c r="I176" s="34"/>
       <c r="J176" s="22"/>
       <c r="K176" s="22"/>
@@ -17107,7 +17132,7 @@
       <c r="N176" s="17"/>
       <c r="O176" s="22"/>
       <c r="P176" s="16"/>
-      <c r="Q176" s="50"/>
+      <c r="Q176" s="49"/>
       <c r="R176" s="17"/>
       <c r="S176" s="17"/>
     </row>
@@ -17118,7 +17143,7 @@
       <c r="E177" s="17"/>
       <c r="F177" s="17"/>
       <c r="G177" s="22"/>
-      <c r="H177" s="50"/>
+      <c r="H177" s="49"/>
       <c r="I177" s="34"/>
       <c r="J177" s="22"/>
       <c r="K177" s="22"/>
@@ -17127,7 +17152,7 @@
       <c r="N177" s="17"/>
       <c r="O177" s="22"/>
       <c r="P177" s="16"/>
-      <c r="Q177" s="50"/>
+      <c r="Q177" s="49"/>
       <c r="R177" s="17"/>
       <c r="S177" s="17"/>
     </row>
@@ -17138,7 +17163,7 @@
       <c r="E178" s="17"/>
       <c r="F178" s="17"/>
       <c r="G178" s="22"/>
-      <c r="H178" s="50"/>
+      <c r="H178" s="49"/>
       <c r="I178" s="34"/>
       <c r="J178" s="22"/>
       <c r="K178" s="22"/>
@@ -17147,7 +17172,7 @@
       <c r="N178" s="17"/>
       <c r="O178" s="22"/>
       <c r="P178" s="16"/>
-      <c r="Q178" s="50"/>
+      <c r="Q178" s="49"/>
       <c r="R178" s="17"/>
       <c r="S178" s="17"/>
     </row>
@@ -17158,7 +17183,7 @@
       <c r="E179" s="17"/>
       <c r="F179" s="17"/>
       <c r="G179" s="22"/>
-      <c r="H179" s="50"/>
+      <c r="H179" s="49"/>
       <c r="I179" s="34"/>
       <c r="J179" s="22"/>
       <c r="K179" s="22"/>
@@ -17167,7 +17192,7 @@
       <c r="N179" s="17"/>
       <c r="O179" s="22"/>
       <c r="P179" s="16"/>
-      <c r="Q179" s="50"/>
+      <c r="Q179" s="49"/>
       <c r="R179" s="17"/>
       <c r="S179" s="17"/>
     </row>
@@ -17178,7 +17203,7 @@
       <c r="E180" s="17"/>
       <c r="F180" s="17"/>
       <c r="G180" s="22"/>
-      <c r="H180" s="50"/>
+      <c r="H180" s="49"/>
       <c r="I180" s="34"/>
       <c r="J180" s="22"/>
       <c r="K180" s="22"/>
@@ -17187,7 +17212,7 @@
       <c r="N180" s="17"/>
       <c r="O180" s="22"/>
       <c r="P180" s="16"/>
-      <c r="Q180" s="50"/>
+      <c r="Q180" s="49"/>
       <c r="R180" s="17"/>
       <c r="S180" s="17"/>
     </row>
@@ -17198,7 +17223,7 @@
       <c r="E181" s="17"/>
       <c r="F181" s="17"/>
       <c r="G181" s="22"/>
-      <c r="H181" s="50"/>
+      <c r="H181" s="49"/>
       <c r="I181" s="34"/>
       <c r="J181" s="22"/>
       <c r="K181" s="22"/>
@@ -17207,7 +17232,7 @@
       <c r="N181" s="17"/>
       <c r="O181" s="22"/>
       <c r="P181" s="16"/>
-      <c r="Q181" s="50"/>
+      <c r="Q181" s="49"/>
       <c r="R181" s="17"/>
       <c r="S181" s="17"/>
     </row>
@@ -17230,7 +17255,7 @@
       <c r="G182" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H182" s="50" t="s">
+      <c r="H182" s="49" t="s">
         <v>116</v>
       </c>
       <c r="I182" s="34" t="s">
@@ -17257,7 +17282,7 @@
       <c r="P182" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="Q182" s="50" t="s">
+      <c r="Q182" s="49" t="s">
         <v>121</v>
       </c>
       <c r="R182" s="17" t="s">
@@ -17274,7 +17299,7 @@
       <c r="E183" s="17"/>
       <c r="F183" s="17"/>
       <c r="G183" s="22"/>
-      <c r="H183" s="50"/>
+      <c r="H183" s="49"/>
       <c r="I183" s="34"/>
       <c r="J183" s="22"/>
       <c r="K183" s="22"/>
@@ -17283,7 +17308,7 @@
       <c r="N183" s="17"/>
       <c r="O183" s="22"/>
       <c r="P183" s="16"/>
-      <c r="Q183" s="50"/>
+      <c r="Q183" s="49"/>
       <c r="R183" s="17"/>
       <c r="S183" s="17"/>
     </row>
@@ -17294,7 +17319,7 @@
       <c r="E184" s="17"/>
       <c r="F184" s="17"/>
       <c r="G184" s="22"/>
-      <c r="H184" s="50"/>
+      <c r="H184" s="49"/>
       <c r="I184" s="34"/>
       <c r="J184" s="22"/>
       <c r="K184" s="22"/>
@@ -17303,7 +17328,7 @@
       <c r="N184" s="17"/>
       <c r="O184" s="22"/>
       <c r="P184" s="16"/>
-      <c r="Q184" s="50"/>
+      <c r="Q184" s="49"/>
       <c r="R184" s="17"/>
       <c r="S184" s="17"/>
     </row>
@@ -17314,7 +17339,7 @@
       <c r="E185" s="17"/>
       <c r="F185" s="17"/>
       <c r="G185" s="22"/>
-      <c r="H185" s="50"/>
+      <c r="H185" s="49"/>
       <c r="I185" s="34"/>
       <c r="J185" s="22"/>
       <c r="K185" s="22"/>
@@ -17323,7 +17348,7 @@
       <c r="N185" s="17"/>
       <c r="O185" s="22"/>
       <c r="P185" s="16"/>
-      <c r="Q185" s="50"/>
+      <c r="Q185" s="49"/>
       <c r="R185" s="17"/>
       <c r="S185" s="17"/>
     </row>
@@ -17334,7 +17359,7 @@
       <c r="E186" s="17"/>
       <c r="F186" s="17"/>
       <c r="G186" s="22"/>
-      <c r="H186" s="50"/>
+      <c r="H186" s="49"/>
       <c r="I186" s="34"/>
       <c r="J186" s="22"/>
       <c r="K186" s="22"/>
@@ -17343,7 +17368,7 @@
       <c r="N186" s="17"/>
       <c r="O186" s="22"/>
       <c r="P186" s="16"/>
-      <c r="Q186" s="50"/>
+      <c r="Q186" s="49"/>
       <c r="R186" s="17"/>
       <c r="S186" s="17"/>
     </row>
@@ -17354,7 +17379,7 @@
       <c r="E187" s="17"/>
       <c r="F187" s="17"/>
       <c r="G187" s="22"/>
-      <c r="H187" s="50"/>
+      <c r="H187" s="49"/>
       <c r="I187" s="34"/>
       <c r="J187" s="22"/>
       <c r="K187" s="22"/>
@@ -17363,7 +17388,7 @@
       <c r="N187" s="17"/>
       <c r="O187" s="22"/>
       <c r="P187" s="16"/>
-      <c r="Q187" s="50"/>
+      <c r="Q187" s="49"/>
       <c r="R187" s="17"/>
       <c r="S187" s="17"/>
     </row>
@@ -17374,7 +17399,7 @@
       <c r="E188" s="17"/>
       <c r="F188" s="17"/>
       <c r="G188" s="22"/>
-      <c r="H188" s="50"/>
+      <c r="H188" s="49"/>
       <c r="I188" s="34"/>
       <c r="J188" s="22"/>
       <c r="K188" s="22"/>
@@ -17383,7 +17408,7 @@
       <c r="N188" s="17"/>
       <c r="O188" s="22"/>
       <c r="P188" s="16"/>
-      <c r="Q188" s="50"/>
+      <c r="Q188" s="49"/>
       <c r="R188" s="17"/>
       <c r="S188" s="17"/>
     </row>
@@ -17394,7 +17419,7 @@
       <c r="E189" s="17"/>
       <c r="F189" s="17"/>
       <c r="G189" s="22"/>
-      <c r="H189" s="50"/>
+      <c r="H189" s="49"/>
       <c r="I189" s="34"/>
       <c r="J189" s="22"/>
       <c r="K189" s="22"/>
@@ -17403,7 +17428,7 @@
       <c r="N189" s="17"/>
       <c r="O189" s="22"/>
       <c r="P189" s="16"/>
-      <c r="Q189" s="50"/>
+      <c r="Q189" s="49"/>
       <c r="R189" s="17"/>
       <c r="S189" s="17"/>
     </row>
@@ -17414,7 +17439,7 @@
       <c r="E190" s="17"/>
       <c r="F190" s="17"/>
       <c r="G190" s="22"/>
-      <c r="H190" s="50"/>
+      <c r="H190" s="49"/>
       <c r="I190" s="34"/>
       <c r="J190" s="22"/>
       <c r="K190" s="22"/>
@@ -17423,7 +17448,7 @@
       <c r="N190" s="17"/>
       <c r="O190" s="22"/>
       <c r="P190" s="16"/>
-      <c r="Q190" s="50"/>
+      <c r="Q190" s="49"/>
       <c r="R190" s="17"/>
       <c r="S190" s="17"/>
     </row>
@@ -17434,7 +17459,7 @@
       <c r="E191" s="17"/>
       <c r="F191" s="17"/>
       <c r="G191" s="22"/>
-      <c r="H191" s="50"/>
+      <c r="H191" s="49"/>
       <c r="I191" s="34"/>
       <c r="J191" s="22"/>
       <c r="K191" s="22"/>
@@ -17443,7 +17468,7 @@
       <c r="N191" s="17"/>
       <c r="O191" s="22"/>
       <c r="P191" s="16"/>
-      <c r="Q191" s="50"/>
+      <c r="Q191" s="49"/>
       <c r="R191" s="17"/>
       <c r="S191" s="17"/>
     </row>
@@ -17466,7 +17491,7 @@
       <c r="G192" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H192" s="50" t="s">
+      <c r="H192" s="49" t="s">
         <v>116</v>
       </c>
       <c r="I192" s="34" t="s">
@@ -17493,7 +17518,7 @@
       <c r="P192" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="Q192" s="50" t="s">
+      <c r="Q192" s="49" t="s">
         <v>121</v>
       </c>
       <c r="R192" s="17" t="s">
@@ -17510,7 +17535,7 @@
       <c r="E193" s="17"/>
       <c r="F193" s="17"/>
       <c r="G193" s="22"/>
-      <c r="H193" s="50"/>
+      <c r="H193" s="49"/>
       <c r="I193" s="34"/>
       <c r="J193" s="22"/>
       <c r="K193" s="22"/>
@@ -17519,7 +17544,7 @@
       <c r="N193" s="17"/>
       <c r="O193" s="22"/>
       <c r="P193" s="16"/>
-      <c r="Q193" s="50"/>
+      <c r="Q193" s="49"/>
       <c r="R193" s="17"/>
       <c r="S193" s="17"/>
     </row>
@@ -20183,7 +20208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V611"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K37" workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>

</xml_diff>